<commit_message>
Flujo de caja emprendimiento completado, retirar la carta gantt despues de exportar a project Actualizacion dato pequeño
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Desarrollo del emprendimiento/Proyecto ABpro Nª2/assets/Flujo de caja.xlsx
+++ b/trabajos.inacap.2019/Desarrollo del emprendimiento/Proyecto ABpro Nª2/assets/Flujo de caja.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458CAB8F-A540-4519-913E-2AF3C12039D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C43CE-D874-45E8-9165-B63CBA568A3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1232,6 +1232,98 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="17" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="19" fillId="6" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="15" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="16" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="17" xfId="19" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="17" borderId="15" xfId="19" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="17" borderId="16" xfId="19" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="17" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="13" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="16" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="17" borderId="17" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="16"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="8" applyFont="1"/>
+    <xf numFmtId="42" fontId="19" fillId="6" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,98 +1363,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="17" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="19" fillId="6" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="18" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="15" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="16" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="17" xfId="19" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="15" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="16" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="13" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="16" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="17" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="16"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="8" applyFont="1"/>
-    <xf numFmtId="42" fontId="19" fillId="6" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="20% - Énfasis1" xfId="9" builtinId="30"/>
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AY38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ6" sqref="AQ6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,65 +1747,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
       <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="2:51" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="95"/>
-      <c r="Q3" s="97" t="s">
+      <c r="B3" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="147"/>
+      <c r="Q3" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="98"/>
-      <c r="Y3" s="102" t="s">
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="116"/>
+      <c r="Y3" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="103"/>
-      <c r="AA3" s="103"/>
-      <c r="AB3" s="103"/>
-      <c r="AC3" s="104"/>
-      <c r="AE3" s="97" t="s">
+      <c r="Z3" s="126"/>
+      <c r="AA3" s="126"/>
+      <c r="AB3" s="126"/>
+      <c r="AC3" s="127"/>
+      <c r="AE3" s="115" t="s">
         <v>134</v>
       </c>
-      <c r="AF3" s="105"/>
-      <c r="AG3" s="105"/>
-      <c r="AH3" s="105"/>
-      <c r="AI3" s="105"/>
-      <c r="AJ3" s="105"/>
-      <c r="AK3" s="105"/>
-      <c r="AL3" s="105"/>
-      <c r="AM3" s="105"/>
-      <c r="AN3" s="105"/>
-      <c r="AO3" s="98"/>
-      <c r="AT3" s="96" t="s">
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
+      <c r="AH3" s="117"/>
+      <c r="AI3" s="117"/>
+      <c r="AJ3" s="117"/>
+      <c r="AK3" s="117"/>
+      <c r="AL3" s="117"/>
+      <c r="AM3" s="117"/>
+      <c r="AN3" s="117"/>
+      <c r="AO3" s="116"/>
+      <c r="AT3" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="AU3" s="96"/>
-      <c r="AV3" s="96"/>
+      <c r="AU3" s="118"/>
+      <c r="AV3" s="118"/>
     </row>
     <row r="4" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1845,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="113" t="s">
+      <c r="Q4" s="87" t="s">
         <v>17</v>
       </c>
       <c r="R4" s="22" t="s">
@@ -1857,77 +1857,77 @@
       <c r="T4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="114" t="s">
+      <c r="U4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="Y4" s="106" t="s">
+      <c r="Y4" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="107"/>
-      <c r="AA4" s="107"/>
-      <c r="AB4" s="107"/>
-      <c r="AC4" s="108"/>
-      <c r="AE4" s="127" t="s">
+      <c r="Z4" s="129"/>
+      <c r="AA4" s="129"/>
+      <c r="AB4" s="129"/>
+      <c r="AC4" s="130"/>
+      <c r="AE4" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="AF4" s="127" t="s">
+      <c r="AF4" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="AG4" s="127" t="s">
+      <c r="AG4" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="AH4" s="127" t="s">
+      <c r="AH4" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="AI4" s="127" t="s">
+      <c r="AI4" s="94" t="s">
         <v>129</v>
       </c>
-      <c r="AJ4" s="127" t="s">
+      <c r="AJ4" s="94" t="s">
         <v>167</v>
       </c>
-      <c r="AK4" s="127" t="s">
+      <c r="AK4" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="AL4" s="127" t="s">
+      <c r="AL4" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="AM4" s="127" t="s">
+      <c r="AM4" s="94" t="s">
         <v>168</v>
       </c>
-      <c r="AN4" s="127" t="s">
+      <c r="AN4" s="94" t="s">
         <v>166</v>
       </c>
-      <c r="AO4" s="127" t="s">
+      <c r="AO4" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="AT4" s="122" t="s">
+      <c r="AT4" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="AU4" s="122" t="s">
+      <c r="AU4" s="89" t="s">
         <v>143</v>
       </c>
-      <c r="AV4" s="122" t="s">
+      <c r="AV4" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="AW4" s="123"/>
-      <c r="AX4" s="123"/>
-      <c r="AY4" s="123"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="90"/>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="85"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="137"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="8" t="s">
         <v>7</v>
@@ -1961,46 +1961,46 @@
       <c r="AC5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AE5" s="131" t="s">
+      <c r="AE5" s="98" t="s">
         <v>132</v>
       </c>
-      <c r="AF5" s="131" t="s">
+      <c r="AF5" s="98" t="s">
         <v>137</v>
       </c>
-      <c r="AG5" s="134">
+      <c r="AG5" s="101">
         <v>43538</v>
       </c>
-      <c r="AH5" s="134">
+      <c r="AH5" s="101">
         <v>43827</v>
       </c>
-      <c r="AI5" s="131"/>
-      <c r="AJ5" s="131">
+      <c r="AI5" s="98"/>
+      <c r="AJ5" s="98">
         <v>7</v>
       </c>
-      <c r="AK5" s="131">
+      <c r="AK5" s="98">
         <v>6</v>
       </c>
-      <c r="AL5" s="128">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="131">
+      <c r="AL5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="98">
         <f>((AH5-AG5)*6)+AL5</f>
         <v>1734</v>
       </c>
-      <c r="AN5" s="138">
+      <c r="AN5" s="105">
         <v>17000</v>
       </c>
-      <c r="AO5" s="137">
+      <c r="AO5" s="104">
         <f>AM5*AN5</f>
         <v>29478000</v>
       </c>
       <c r="AT5" t="s">
         <v>145</v>
       </c>
-      <c r="AU5" s="126">
+      <c r="AU5" s="93">
         <v>43538</v>
       </c>
-      <c r="AV5" s="126">
+      <c r="AV5" s="93">
         <v>43545</v>
       </c>
     </row>
@@ -2073,46 +2073,46 @@
         <f t="shared" ref="AC6:AC12" si="1">AA6*AB6</f>
         <v>3879960</v>
       </c>
-      <c r="AE6" s="132" t="s">
+      <c r="AE6" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF6" s="132" t="s">
+      <c r="AF6" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="AG6" s="135">
+      <c r="AG6" s="102">
         <v>43539</v>
       </c>
-      <c r="AH6" s="135">
+      <c r="AH6" s="102">
         <v>43827</v>
       </c>
-      <c r="AI6" s="132"/>
-      <c r="AJ6" s="132">
+      <c r="AI6" s="99"/>
+      <c r="AJ6" s="99">
         <v>7</v>
       </c>
-      <c r="AK6" s="132">
+      <c r="AK6" s="99">
         <v>6</v>
       </c>
-      <c r="AL6" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="132">
+      <c r="AL6" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="99">
         <f t="shared" ref="AM6:AM24" si="2">((AH6-AG6)*6)+AL6</f>
         <v>1728</v>
       </c>
-      <c r="AN6" s="139">
+      <c r="AN6" s="106">
         <v>16500</v>
       </c>
-      <c r="AO6" s="141">
+      <c r="AO6" s="108">
         <f t="shared" ref="AO6:AO24" si="3">AM6*AN6</f>
         <v>28512000</v>
       </c>
       <c r="AT6" t="s">
         <v>146</v>
       </c>
-      <c r="AU6" s="126">
+      <c r="AU6" s="93">
         <v>43525</v>
       </c>
-      <c r="AV6" s="126">
+      <c r="AV6" s="93">
         <v>43532</v>
       </c>
     </row>
@@ -2194,46 +2194,46 @@
         <f t="shared" si="1"/>
         <v>86990</v>
       </c>
-      <c r="AE7" s="132" t="s">
+      <c r="AE7" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF7" s="132" t="s">
+      <c r="AF7" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="AG7" s="135">
+      <c r="AG7" s="102">
         <v>43560</v>
       </c>
-      <c r="AH7" s="135">
+      <c r="AH7" s="102">
         <v>43827</v>
       </c>
-      <c r="AI7" s="132"/>
-      <c r="AJ7" s="132">
+      <c r="AI7" s="99"/>
+      <c r="AJ7" s="99">
         <v>7</v>
       </c>
-      <c r="AK7" s="132">
+      <c r="AK7" s="99">
         <v>6</v>
       </c>
-      <c r="AL7" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="132">
+      <c r="AL7" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="99">
         <f t="shared" si="2"/>
         <v>1602</v>
       </c>
-      <c r="AN7" s="139">
+      <c r="AN7" s="106">
         <v>15000</v>
       </c>
-      <c r="AO7" s="141">
+      <c r="AO7" s="108">
         <f t="shared" si="3"/>
         <v>24030000</v>
       </c>
       <c r="AT7" t="s">
         <v>147</v>
       </c>
-      <c r="AU7" s="126">
+      <c r="AU7" s="93">
         <v>43533</v>
       </c>
-      <c r="AV7" s="126">
+      <c r="AV7" s="93">
         <v>43559</v>
       </c>
     </row>
@@ -2242,47 +2242,47 @@
         <v>110</v>
       </c>
       <c r="C8" s="17">
-        <f>$L$29*C7</f>
+        <f t="shared" ref="C8:M8" si="5">$L$29*C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="17">
-        <f>$L$29*D7</f>
+        <f t="shared" si="5"/>
         <v>130925500</v>
       </c>
       <c r="E8" s="17">
-        <f>$L$29*E7</f>
+        <f t="shared" si="5"/>
         <v>261851000</v>
       </c>
       <c r="F8" s="17">
-        <f>$L$29*F7</f>
+        <f t="shared" si="5"/>
         <v>392776499.99999994</v>
       </c>
       <c r="G8" s="17">
-        <f>$L$29*G7</f>
+        <f t="shared" si="5"/>
         <v>523702000</v>
       </c>
       <c r="H8" s="17">
-        <f>$L$29*H7</f>
+        <f t="shared" si="5"/>
         <v>654627500</v>
       </c>
       <c r="I8" s="17">
-        <f>$L$29*I7</f>
+        <f t="shared" si="5"/>
         <v>785552999.99999988</v>
       </c>
       <c r="J8" s="17">
-        <f>$L$29*J7</f>
+        <f t="shared" si="5"/>
         <v>916478499.99999988</v>
       </c>
       <c r="K8" s="17">
-        <f>$L$29*K7</f>
+        <f t="shared" si="5"/>
         <v>1047403999.9999998</v>
       </c>
       <c r="L8" s="17">
-        <f>$L$29*L7</f>
+        <f t="shared" si="5"/>
         <v>1178329499.9999998</v>
       </c>
       <c r="M8" s="76">
-        <f>$L$29*M7</f>
+        <f t="shared" si="5"/>
         <v>1309254999.9999998</v>
       </c>
       <c r="P8" s="6"/>
@@ -2316,46 +2316,46 @@
         <f t="shared" si="1"/>
         <v>581960</v>
       </c>
-      <c r="AE8" s="132" t="s">
+      <c r="AE8" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF8" s="132" t="s">
+      <c r="AF8" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG8" s="135">
+      <c r="AG8" s="102">
         <v>43588</v>
       </c>
-      <c r="AH8" s="135">
+      <c r="AH8" s="102">
         <v>43827</v>
       </c>
-      <c r="AI8" s="132"/>
-      <c r="AJ8" s="132">
+      <c r="AI8" s="99"/>
+      <c r="AJ8" s="99">
         <v>7</v>
       </c>
-      <c r="AK8" s="132">
+      <c r="AK8" s="99">
         <v>6</v>
       </c>
-      <c r="AL8" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="132">
+      <c r="AL8" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN8" s="139">
+      <c r="AN8" s="106">
         <v>14000</v>
       </c>
-      <c r="AO8" s="141">
+      <c r="AO8" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT8" t="s">
         <v>148</v>
       </c>
-      <c r="AU8" s="126">
+      <c r="AU8" s="93">
         <v>43560</v>
       </c>
-      <c r="AV8" s="126">
+      <c r="AV8" s="93">
         <v>43595</v>
       </c>
     </row>
@@ -2372,39 +2372,39 @@
         <v>130925500</v>
       </c>
       <c r="E9" s="77">
-        <f t="shared" ref="E9:M9" si="5">E8</f>
+        <f t="shared" ref="E9:M9" si="6">E8</f>
         <v>261851000</v>
       </c>
       <c r="F9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>392776499.99999994</v>
       </c>
       <c r="G9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>523702000</v>
       </c>
       <c r="H9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>654627500</v>
       </c>
       <c r="I9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>785552999.99999988</v>
       </c>
       <c r="J9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>916478499.99999988</v>
       </c>
       <c r="K9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1047403999.9999998</v>
       </c>
       <c r="L9" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1178329499.9999998</v>
       </c>
       <c r="M9" s="78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1309254999.9999998</v>
       </c>
       <c r="P9" s="6"/>
@@ -2438,46 +2438,46 @@
         <f t="shared" si="1"/>
         <v>279090</v>
       </c>
-      <c r="AE9" s="132" t="s">
+      <c r="AE9" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF9" s="132" t="s">
+      <c r="AF9" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG9" s="135">
+      <c r="AG9" s="102">
         <v>43588</v>
       </c>
-      <c r="AH9" s="135">
+      <c r="AH9" s="102">
         <v>43827</v>
       </c>
-      <c r="AI9" s="132"/>
-      <c r="AJ9" s="132">
+      <c r="AI9" s="99"/>
+      <c r="AJ9" s="99">
         <v>7</v>
       </c>
-      <c r="AK9" s="132">
+      <c r="AK9" s="99">
         <v>6</v>
       </c>
-      <c r="AL9" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="132">
+      <c r="AL9" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN9" s="139">
+      <c r="AN9" s="106">
         <v>14000</v>
       </c>
-      <c r="AO9" s="141">
+      <c r="AO9" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT9" t="s">
         <v>150</v>
       </c>
-      <c r="AU9" s="126">
+      <c r="AU9" s="93">
         <v>43596</v>
       </c>
-      <c r="AV9" s="126">
+      <c r="AV9" s="93">
         <v>43617</v>
       </c>
     </row>
@@ -2489,43 +2489,43 @@
         <v>0</v>
       </c>
       <c r="D10" s="79">
-        <f>D9-(D9*$L$38)</f>
+        <f t="shared" ref="D10:M10" si="7">D9-(D9*$L$38)</f>
         <v>95575615</v>
       </c>
       <c r="E10" s="79">
-        <f>E9-(E9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>191151230</v>
       </c>
       <c r="F10" s="79">
-        <f>F9-(F9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>286726844.99999994</v>
       </c>
       <c r="G10" s="79">
-        <f>G9-(G9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>382302460</v>
       </c>
       <c r="H10" s="79">
-        <f>H9-(H9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>477878075</v>
       </c>
       <c r="I10" s="79">
-        <f>I9-(I9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>573453689.99999988</v>
       </c>
       <c r="J10" s="79">
-        <f>J9-(J9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>669029304.99999988</v>
       </c>
       <c r="K10" s="79">
-        <f>K9-(K9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>764604919.99999976</v>
       </c>
       <c r="L10" s="79">
-        <f>L9-(L9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>860180534.99999976</v>
       </c>
       <c r="M10" s="80">
-        <f>M9-(M9*$L$38)</f>
+        <f t="shared" si="7"/>
         <v>955756149.99999976</v>
       </c>
       <c r="P10" s="6"/>
@@ -2559,46 +2559,46 @@
         <f t="shared" si="1"/>
         <v>99800</v>
       </c>
-      <c r="AE10" s="132" t="s">
+      <c r="AE10" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF10" s="132" t="s">
+      <c r="AF10" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG10" s="135">
+      <c r="AG10" s="102">
         <v>43588</v>
       </c>
-      <c r="AH10" s="135">
+      <c r="AH10" s="102">
         <v>43827</v>
       </c>
-      <c r="AI10" s="132"/>
-      <c r="AJ10" s="132">
+      <c r="AI10" s="99"/>
+      <c r="AJ10" s="99">
         <v>7</v>
       </c>
-      <c r="AK10" s="132">
+      <c r="AK10" s="99">
         <v>6</v>
       </c>
-      <c r="AL10" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="132">
+      <c r="AL10" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN10" s="139">
+      <c r="AN10" s="106">
         <v>14000</v>
       </c>
-      <c r="AO10" s="141">
+      <c r="AO10" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT10" t="s">
         <v>156</v>
       </c>
-      <c r="AU10" s="126">
+      <c r="AU10" s="93">
         <v>43618</v>
       </c>
-      <c r="AV10" s="126">
+      <c r="AV10" s="93">
         <v>43623</v>
       </c>
     </row>
@@ -2625,64 +2625,64 @@
         <f t="shared" si="1"/>
         <v>1899800</v>
       </c>
-      <c r="AE11" s="132" t="s">
+      <c r="AE11" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF11" s="132" t="s">
+      <c r="AF11" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG11" s="135">
+      <c r="AG11" s="102">
         <v>43588</v>
       </c>
-      <c r="AH11" s="135">
+      <c r="AH11" s="102">
         <v>43827</v>
       </c>
-      <c r="AI11" s="132"/>
-      <c r="AJ11" s="132">
+      <c r="AI11" s="99"/>
+      <c r="AJ11" s="99">
         <v>7</v>
       </c>
-      <c r="AK11" s="132">
+      <c r="AK11" s="99">
         <v>6</v>
       </c>
-      <c r="AL11" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="132">
+      <c r="AL11" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN11" s="139">
+      <c r="AN11" s="106">
         <v>14000</v>
       </c>
-      <c r="AO11" s="141">
+      <c r="AO11" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT11" t="s">
         <v>149</v>
       </c>
-      <c r="AU11" s="126">
+      <c r="AU11" s="93">
         <v>43624</v>
       </c>
-      <c r="AV11" s="126">
+      <c r="AV11" s="93">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="88"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="140"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -2691,7 +2691,7 @@
       <c r="Y12" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="Z12" s="145" t="s">
+      <c r="Z12" s="112" t="s">
         <v>170</v>
       </c>
       <c r="AA12" s="38">
@@ -2704,46 +2704,46 @@
         <f t="shared" si="1"/>
         <v>10669800</v>
       </c>
-      <c r="AE12" s="132" t="s">
+      <c r="AE12" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF12" s="132" t="s">
+      <c r="AF12" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG12" s="135">
+      <c r="AG12" s="102">
         <v>43588</v>
       </c>
-      <c r="AH12" s="135">
+      <c r="AH12" s="102">
         <v>43827</v>
       </c>
-      <c r="AI12" s="132"/>
-      <c r="AJ12" s="132">
+      <c r="AI12" s="99"/>
+      <c r="AJ12" s="99">
         <v>7</v>
       </c>
-      <c r="AK12" s="132">
+      <c r="AK12" s="99">
         <v>6</v>
       </c>
-      <c r="AL12" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="132">
+      <c r="AL12" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN12" s="139">
+      <c r="AN12" s="106">
         <v>14000</v>
       </c>
-      <c r="AO12" s="141">
+      <c r="AO12" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT12" t="s">
         <v>151</v>
       </c>
-      <c r="AU12" s="126">
+      <c r="AU12" s="93">
         <v>43625</v>
       </c>
-      <c r="AV12" s="126">
+      <c r="AV12" s="93">
         <v>43645</v>
       </c>
     </row>
@@ -2759,54 +2759,54 @@
         <v>145495480.56</v>
       </c>
       <c r="E13" s="74">
-        <f t="shared" ref="E13:M13" si="6">$U$5*12</f>
+        <f t="shared" ref="E13:M13" si="8">$U$5*12</f>
         <v>145495480.56</v>
       </c>
       <c r="F13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="G13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="H13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="I13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="J13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="K13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="L13" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
       <c r="M13" s="75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>145495480.56</v>
       </c>
-      <c r="Q13" s="111" t="s">
+      <c r="Q13" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="109" t="s">
+      <c r="R13" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="S13" s="109" t="s">
+      <c r="S13" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="T13" s="109" t="s">
+      <c r="T13" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="U13" s="110" t="s">
+      <c r="U13" s="84" t="s">
         <v>19</v>
       </c>
       <c r="Y13" s="8"/>
@@ -2819,46 +2819,46 @@
         <f>SUM(AC6:AC12)</f>
         <v>17497400</v>
       </c>
-      <c r="AE13" s="132" t="s">
+      <c r="AE13" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF13" s="132" t="s">
+      <c r="AF13" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG13" s="135">
+      <c r="AG13" s="102">
         <v>43588</v>
       </c>
-      <c r="AH13" s="135">
+      <c r="AH13" s="102">
         <v>43827</v>
       </c>
-      <c r="AI13" s="132"/>
-      <c r="AJ13" s="132">
+      <c r="AI13" s="99"/>
+      <c r="AJ13" s="99">
         <v>7</v>
       </c>
-      <c r="AK13" s="132">
+      <c r="AK13" s="99">
         <v>6</v>
       </c>
-      <c r="AL13" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="132">
+      <c r="AL13" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN13" s="139">
+      <c r="AN13" s="106">
         <v>14000</v>
       </c>
-      <c r="AO13" s="141">
+      <c r="AO13" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT13" t="s">
         <v>159</v>
       </c>
-      <c r="AU13" s="126">
+      <c r="AU13" s="93">
         <v>43646</v>
       </c>
-      <c r="AV13" s="126">
+      <c r="AV13" s="93">
         <v>43651</v>
       </c>
     </row>
@@ -2870,109 +2870,109 @@
         <v>12</v>
       </c>
       <c r="D14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" ref="D14:M14" si="9">$U$14*12</f>
+        <v>2964000</v>
       </c>
       <c r="E14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="F14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="G14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="H14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="I14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="J14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="K14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="L14" s="17">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="M14" s="76">
-        <f>$U$14*12</f>
-        <v>1716000</v>
+        <f t="shared" si="9"/>
+        <v>2964000</v>
       </c>
       <c r="Q14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="R14" s="13">
-        <v>80000</v>
+        <v>120000</v>
       </c>
       <c r="S14" s="51">
         <v>0.3</v>
       </c>
       <c r="T14" s="13">
         <f>(R14*S14)+R14</f>
-        <v>104000</v>
-      </c>
-      <c r="U14" s="112">
+        <v>156000</v>
+      </c>
+      <c r="U14" s="86">
         <f>SUM(T14:T15)</f>
-        <v>143000</v>
-      </c>
-      <c r="Y14" s="89" t="s">
+        <v>247000</v>
+      </c>
+      <c r="Y14" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="Z14" s="90"/>
-      <c r="AA14" s="90"/>
-      <c r="AB14" s="90"/>
-      <c r="AC14" s="91"/>
-      <c r="AE14" s="132" t="s">
+      <c r="Z14" s="142"/>
+      <c r="AA14" s="142"/>
+      <c r="AB14" s="142"/>
+      <c r="AC14" s="143"/>
+      <c r="AE14" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF14" s="132" t="s">
+      <c r="AF14" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG14" s="135">
+      <c r="AG14" s="102">
         <v>43588</v>
       </c>
-      <c r="AH14" s="135">
+      <c r="AH14" s="102">
         <v>43827</v>
       </c>
-      <c r="AI14" s="132"/>
-      <c r="AJ14" s="132">
+      <c r="AI14" s="99"/>
+      <c r="AJ14" s="99">
         <v>7</v>
       </c>
-      <c r="AK14" s="132">
+      <c r="AK14" s="99">
         <v>6</v>
       </c>
-      <c r="AL14" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="132">
+      <c r="AL14" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN14" s="139">
+      <c r="AN14" s="106">
         <v>14000</v>
       </c>
-      <c r="AO14" s="141">
+      <c r="AO14" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT14" t="s">
         <v>152</v>
       </c>
-      <c r="AU14" s="126">
+      <c r="AU14" s="93">
         <v>43652</v>
       </c>
-      <c r="AV14" s="126">
+      <c r="AV14" s="93">
         <v>43652</v>
       </c>
     </row>
@@ -2984,27 +2984,27 @@
         <v>12</v>
       </c>
       <c r="D15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" ref="D15:I15" si="10">$AC$13/6</f>
         <v>2916233.3333333335</v>
       </c>
       <c r="E15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" si="10"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="F15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" si="10"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="G15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" si="10"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="H15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" si="10"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="I15" s="17">
-        <f>$AC$13/6</f>
+        <f t="shared" si="10"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="J15" s="17">
@@ -3023,14 +3023,14 @@
         <v>5</v>
       </c>
       <c r="R15" s="13">
-        <v>30000</v>
+        <v>70000</v>
       </c>
       <c r="S15" s="51">
         <v>0.3</v>
       </c>
       <c r="T15" s="13">
-        <f t="shared" ref="T15" si="7">(R15*S15)+R15</f>
-        <v>39000</v>
+        <f t="shared" ref="T15" si="11">(R15*S15)+R15</f>
+        <v>91000</v>
       </c>
       <c r="U15" s="7"/>
       <c r="Y15" s="27" t="s">
@@ -3048,46 +3048,46 @@
       <c r="AC15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="AE15" s="132" t="s">
+      <c r="AE15" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF15" s="132" t="s">
+      <c r="AF15" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG15" s="135">
+      <c r="AG15" s="102">
         <v>43588</v>
       </c>
-      <c r="AH15" s="135">
+      <c r="AH15" s="102">
         <v>43827</v>
       </c>
-      <c r="AI15" s="132"/>
-      <c r="AJ15" s="132">
+      <c r="AI15" s="99"/>
+      <c r="AJ15" s="99">
         <v>7</v>
       </c>
-      <c r="AK15" s="132">
+      <c r="AK15" s="99">
         <v>6</v>
       </c>
-      <c r="AL15" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM15" s="132">
+      <c r="AL15" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN15" s="139">
+      <c r="AN15" s="106">
         <v>14000</v>
       </c>
-      <c r="AO15" s="141">
+      <c r="AO15" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT15" t="s">
         <v>153</v>
       </c>
-      <c r="AU15" s="126">
+      <c r="AU15" s="93">
         <v>43653</v>
       </c>
-      <c r="AV15" s="126">
+      <c r="AV15" s="93">
         <v>43676</v>
       </c>
     </row>
@@ -3099,31 +3099,31 @@
         <v>12</v>
       </c>
       <c r="D16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" ref="D16:J16" si="12">$AC$25/7</f>
         <v>1097028.5714285714</v>
       </c>
       <c r="E16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="F16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="G16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="H16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="I16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="J16" s="17">
-        <f>$AC$25/7</f>
+        <f t="shared" si="12"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="K16" s="17">
@@ -3156,46 +3156,46 @@
         <f>AA16*AB16</f>
         <v>1639800</v>
       </c>
-      <c r="AE16" s="132" t="s">
+      <c r="AE16" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF16" s="132" t="s">
+      <c r="AF16" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="AG16" s="135">
+      <c r="AG16" s="102">
         <v>43588</v>
       </c>
-      <c r="AH16" s="135">
+      <c r="AH16" s="102">
         <v>43827</v>
       </c>
-      <c r="AI16" s="132"/>
-      <c r="AJ16" s="132">
+      <c r="AI16" s="99"/>
+      <c r="AJ16" s="99">
         <v>7</v>
       </c>
-      <c r="AK16" s="132">
+      <c r="AK16" s="99">
         <v>6</v>
       </c>
-      <c r="AL16" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="132">
+      <c r="AL16" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN16" s="139">
+      <c r="AN16" s="106">
         <v>14000</v>
       </c>
-      <c r="AO16" s="141">
+      <c r="AO16" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT16" t="s">
         <v>158</v>
       </c>
-      <c r="AU16" s="126">
+      <c r="AU16" s="93">
         <v>43677</v>
       </c>
-      <c r="AV16" s="126">
+      <c r="AV16" s="93">
         <v>43682</v>
       </c>
     </row>
@@ -3207,23 +3207,23 @@
         <v>12</v>
       </c>
       <c r="D17" s="17">
-        <f>S27</f>
+        <f t="shared" ref="D17:H18" si="13">S27</f>
         <v>12000000</v>
       </c>
       <c r="E17" s="17">
-        <f>T27</f>
+        <f t="shared" si="13"/>
         <v>9670928.1228583995</v>
       </c>
       <c r="F17" s="17">
-        <f>U27</f>
+        <f t="shared" si="13"/>
         <v>7306920.1675596759</v>
       </c>
       <c r="G17" s="17">
-        <f>V27</f>
+        <f t="shared" si="13"/>
         <v>4907452.0929314708</v>
       </c>
       <c r="H17" s="17">
-        <f>W27</f>
+        <f t="shared" si="13"/>
         <v>2471991.9971838421</v>
       </c>
       <c r="I17" s="17">
@@ -3262,46 +3262,46 @@
         <f>AA17*AB17</f>
         <v>1599800</v>
       </c>
-      <c r="AE17" s="132" t="s">
+      <c r="AE17" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF17" s="132" t="s">
+      <c r="AF17" s="99" t="s">
         <v>164</v>
       </c>
-      <c r="AG17" s="135">
+      <c r="AG17" s="102">
         <v>43588</v>
       </c>
-      <c r="AH17" s="135">
+      <c r="AH17" s="102">
         <v>43827</v>
       </c>
-      <c r="AI17" s="132"/>
-      <c r="AJ17" s="132">
+      <c r="AI17" s="99"/>
+      <c r="AJ17" s="99">
         <v>7</v>
       </c>
-      <c r="AK17" s="132">
+      <c r="AK17" s="99">
         <v>6</v>
       </c>
-      <c r="AL17" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="132">
+      <c r="AL17" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN17" s="139">
+      <c r="AN17" s="106">
         <v>15000</v>
       </c>
-      <c r="AO17" s="141">
+      <c r="AO17" s="108">
         <f t="shared" si="3"/>
         <v>21510000</v>
       </c>
       <c r="AT17" t="s">
         <v>154</v>
       </c>
-      <c r="AU17" s="126">
+      <c r="AU17" s="93">
         <v>43683</v>
       </c>
-      <c r="AV17" s="126">
+      <c r="AV17" s="93">
         <v>43683</v>
       </c>
     </row>
@@ -3313,23 +3313,23 @@
         <v>12</v>
       </c>
       <c r="D18" s="17">
-        <f>S28</f>
+        <f t="shared" si="13"/>
         <v>155271458.4761067</v>
       </c>
       <c r="E18" s="17">
-        <f>T28</f>
+        <f t="shared" si="13"/>
         <v>157600530.3532483</v>
       </c>
       <c r="F18" s="17">
-        <f>U28</f>
+        <f t="shared" si="13"/>
         <v>159964538.30854702</v>
       </c>
       <c r="G18" s="17">
-        <f>V28</f>
+        <f t="shared" si="13"/>
         <v>162364006.38317522</v>
       </c>
       <c r="H18" s="17">
-        <f>W28</f>
+        <f t="shared" si="13"/>
         <v>164799466.47892287</v>
       </c>
       <c r="I18" s="17">
@@ -3368,46 +3368,46 @@
         <f>AA18*AB18</f>
         <v>599980</v>
       </c>
-      <c r="AE18" s="132" t="s">
+      <c r="AE18" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF18" s="132" t="s">
+      <c r="AF18" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="AG18" s="135">
+      <c r="AG18" s="102">
         <v>43588</v>
       </c>
-      <c r="AH18" s="135">
+      <c r="AH18" s="102">
         <v>43827</v>
       </c>
-      <c r="AI18" s="132"/>
-      <c r="AJ18" s="132">
+      <c r="AI18" s="99"/>
+      <c r="AJ18" s="99">
         <v>7</v>
       </c>
-      <c r="AK18" s="132">
+      <c r="AK18" s="99">
         <v>6</v>
       </c>
-      <c r="AL18" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="132">
+      <c r="AL18" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN18" s="139">
+      <c r="AN18" s="106">
         <v>14000</v>
       </c>
-      <c r="AO18" s="141">
+      <c r="AO18" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT18" t="s">
         <v>155</v>
       </c>
-      <c r="AU18" s="126">
+      <c r="AU18" s="93">
         <v>43684</v>
       </c>
-      <c r="AV18" s="126">
+      <c r="AV18" s="93">
         <v>43707</v>
       </c>
     </row>
@@ -3467,49 +3467,49 @@
         <v>2</v>
       </c>
       <c r="AC19" s="42">
-        <f t="shared" ref="AC19:AC21" si="8">AA19*AB19</f>
+        <f t="shared" ref="AC19:AC21" si="14">AA19*AB19</f>
         <v>59980</v>
       </c>
-      <c r="AE19" s="132" t="s">
+      <c r="AE19" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF19" s="132" t="s">
+      <c r="AF19" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="AG19" s="135">
+      <c r="AG19" s="102">
         <v>43588</v>
       </c>
-      <c r="AH19" s="135">
+      <c r="AH19" s="102">
         <v>43827</v>
       </c>
-      <c r="AI19" s="132"/>
-      <c r="AJ19" s="132">
+      <c r="AI19" s="99"/>
+      <c r="AJ19" s="99">
         <v>7</v>
       </c>
-      <c r="AK19" s="132">
+      <c r="AK19" s="99">
         <v>6</v>
       </c>
-      <c r="AL19" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="132">
+      <c r="AL19" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN19" s="139">
+      <c r="AN19" s="106">
         <v>14000</v>
       </c>
-      <c r="AO19" s="141">
+      <c r="AO19" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT19" t="s">
         <v>157</v>
       </c>
-      <c r="AU19" s="126">
+      <c r="AU19" s="93">
         <v>43708</v>
       </c>
-      <c r="AV19" s="126">
+      <c r="AV19" s="93">
         <v>43718</v>
       </c>
     </row>
@@ -3569,49 +3569,49 @@
         <v>8</v>
       </c>
       <c r="AC20" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>639920</v>
       </c>
-      <c r="AE20" s="132" t="s">
+      <c r="AE20" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF20" s="132" t="s">
+      <c r="AF20" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="AG20" s="135">
+      <c r="AG20" s="102">
         <v>43588</v>
       </c>
-      <c r="AH20" s="135">
+      <c r="AH20" s="102">
         <v>43827</v>
       </c>
-      <c r="AI20" s="132"/>
-      <c r="AJ20" s="132">
+      <c r="AI20" s="99"/>
+      <c r="AJ20" s="99">
         <v>7</v>
       </c>
-      <c r="AK20" s="132">
+      <c r="AK20" s="99">
         <v>6</v>
       </c>
-      <c r="AL20" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="132">
+      <c r="AL20" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN20" s="139">
+      <c r="AN20" s="106">
         <v>15000</v>
       </c>
-      <c r="AO20" s="141">
+      <c r="AO20" s="108">
         <f t="shared" si="3"/>
         <v>21510000</v>
       </c>
       <c r="AT20" t="s">
         <v>160</v>
       </c>
-      <c r="AU20" s="126">
+      <c r="AU20" s="93">
         <v>43719</v>
       </c>
-      <c r="AV20" s="126">
+      <c r="AV20" s="93">
         <v>43748</v>
       </c>
     </row>
@@ -3666,49 +3666,49 @@
         <v>2</v>
       </c>
       <c r="AC21" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>139980</v>
       </c>
-      <c r="AE21" s="132" t="s">
+      <c r="AE21" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF21" s="132" t="s">
+      <c r="AF21" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="AG21" s="135">
+      <c r="AG21" s="102">
         <v>43588</v>
       </c>
-      <c r="AH21" s="135">
+      <c r="AH21" s="102">
         <v>43827</v>
       </c>
-      <c r="AI21" s="132"/>
-      <c r="AJ21" s="132">
+      <c r="AI21" s="99"/>
+      <c r="AJ21" s="99">
         <v>7</v>
       </c>
-      <c r="AK21" s="132">
+      <c r="AK21" s="99">
         <v>6</v>
       </c>
-      <c r="AL21" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="132">
+      <c r="AL21" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN21" s="139">
+      <c r="AN21" s="106">
         <v>14000</v>
       </c>
-      <c r="AO21" s="141">
+      <c r="AO21" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT21" t="s">
         <v>161</v>
       </c>
-      <c r="AU21" s="126">
+      <c r="AU21" s="93">
         <v>43749</v>
       </c>
-      <c r="AV21" s="126">
+      <c r="AV21" s="93">
         <v>43827</v>
       </c>
     </row>
@@ -3750,10 +3750,10 @@
       <c r="M22" s="68">
         <v>0</v>
       </c>
-      <c r="Q22" s="115" t="s">
+      <c r="Q22" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="R22" s="115"/>
+      <c r="R22" s="131"/>
       <c r="Y22" s="40" t="s">
         <v>55</v>
       </c>
@@ -3770,43 +3770,43 @@
         <f>AA22*AB22</f>
         <v>1599980</v>
       </c>
-      <c r="AE22" s="132" t="s">
+      <c r="AE22" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF22" s="132" t="s">
+      <c r="AF22" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="AG22" s="135">
+      <c r="AG22" s="102">
         <v>43588</v>
       </c>
-      <c r="AH22" s="135">
+      <c r="AH22" s="102">
         <v>43827</v>
       </c>
-      <c r="AI22" s="132"/>
-      <c r="AJ22" s="132">
+      <c r="AI22" s="99"/>
+      <c r="AJ22" s="99">
         <v>7</v>
       </c>
-      <c r="AK22" s="132">
+      <c r="AK22" s="99">
         <v>6</v>
       </c>
-      <c r="AL22" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="132">
+      <c r="AL22" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="99">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN22" s="139">
+      <c r="AN22" s="106">
         <v>14000</v>
       </c>
-      <c r="AO22" s="141">
+      <c r="AO22" s="108">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
       <c r="AT22" t="s">
         <v>162</v>
       </c>
-      <c r="AU22" s="126">
+      <c r="AU22" s="93">
         <v>43828</v>
       </c>
     </row>
@@ -3827,36 +3827,36 @@
         <f>AA23*AB23</f>
         <v>799960</v>
       </c>
-      <c r="AE23" s="132" t="s">
+      <c r="AE23" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="AF23" s="132" t="s">
+      <c r="AF23" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="AG23" s="135">
+      <c r="AG23" s="102">
         <v>43719</v>
       </c>
-      <c r="AH23" s="135">
+      <c r="AH23" s="102">
         <v>43827</v>
       </c>
-      <c r="AI23" s="132"/>
-      <c r="AJ23" s="132">
+      <c r="AI23" s="99"/>
+      <c r="AJ23" s="99">
         <v>7</v>
       </c>
-      <c r="AK23" s="132">
+      <c r="AK23" s="99">
         <v>6</v>
       </c>
-      <c r="AL23" s="129">
-        <v>0</v>
-      </c>
-      <c r="AM23" s="132">
+      <c r="AL23" s="96">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="99">
         <f t="shared" si="2"/>
         <v>648</v>
       </c>
-      <c r="AN23" s="139">
+      <c r="AN23" s="106">
         <v>14000</v>
       </c>
-      <c r="AO23" s="141">
+      <c r="AO23" s="108">
         <f t="shared" si="3"/>
         <v>9072000</v>
       </c>
@@ -3876,15 +3876,15 @@
       <c r="K24" s="120"/>
       <c r="L24" s="120"/>
       <c r="M24" s="121"/>
-      <c r="Q24" s="97" t="s">
+      <c r="Q24" s="115" t="s">
         <v>103</v>
       </c>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
-      <c r="W24" s="98"/>
+      <c r="R24" s="117"/>
+      <c r="S24" s="117"/>
+      <c r="T24" s="117"/>
+      <c r="U24" s="117"/>
+      <c r="V24" s="117"/>
+      <c r="W24" s="116"/>
       <c r="Y24" s="40" t="s">
         <v>59</v>
       </c>
@@ -3901,36 +3901,36 @@
         <f>AA24*AB24</f>
         <v>599800</v>
       </c>
-      <c r="AE24" s="133" t="s">
+      <c r="AE24" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="AF24" s="133" t="s">
+      <c r="AF24" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="AG24" s="136">
+      <c r="AG24" s="103">
         <v>43719</v>
       </c>
-      <c r="AH24" s="136">
+      <c r="AH24" s="103">
         <v>43827</v>
       </c>
-      <c r="AI24" s="133"/>
-      <c r="AJ24" s="133">
+      <c r="AI24" s="100"/>
+      <c r="AJ24" s="100">
         <v>7</v>
       </c>
-      <c r="AK24" s="133">
+      <c r="AK24" s="100">
         <v>6</v>
       </c>
-      <c r="AL24" s="130">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="133">
+      <c r="AL24" s="97">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="100">
         <f t="shared" si="2"/>
         <v>648</v>
       </c>
-      <c r="AN24" s="140">
+      <c r="AN24" s="107">
         <v>14000</v>
       </c>
-      <c r="AO24" s="142">
+      <c r="AO24" s="109">
         <f t="shared" si="3"/>
         <v>9072000</v>
       </c>
@@ -3939,49 +3939,49 @@
       <c r="B25" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="124">
+      <c r="C25" s="91">
         <f>C6-C19-C20-C21-C22</f>
         <v>369912992</v>
       </c>
-      <c r="D25" s="124">
+      <c r="D25" s="91">
         <f>D10-SUM(D13,D14,D18,D19,D20,D21,D22)</f>
-        <v>-206907324.03610671</v>
-      </c>
-      <c r="E25" s="124">
-        <f t="shared" ref="E25:M25" si="9">E10-SUM(E13,E14,E18,E19,E20,E21,E22)</f>
-        <v>-113660780.9132483</v>
-      </c>
-      <c r="F25" s="124">
-        <f t="shared" si="9"/>
-        <v>-20449173.868547082</v>
-      </c>
-      <c r="G25" s="124">
-        <f t="shared" si="9"/>
-        <v>72726973.056824803</v>
-      </c>
-      <c r="H25" s="124">
-        <f t="shared" si="9"/>
-        <v>165867127.96107709</v>
-      </c>
-      <c r="I25" s="124">
-        <f t="shared" si="9"/>
-        <v>426242209.43999988</v>
-      </c>
-      <c r="J25" s="124">
-        <f t="shared" si="9"/>
-        <v>521817824.43999988</v>
-      </c>
-      <c r="K25" s="124">
-        <f t="shared" si="9"/>
-        <v>617393439.43999982</v>
-      </c>
-      <c r="L25" s="124">
-        <f t="shared" si="9"/>
-        <v>712969054.43999982</v>
-      </c>
-      <c r="M25" s="124">
-        <f t="shared" si="9"/>
-        <v>808544669.43999982</v>
+        <v>-208155324.03610671</v>
+      </c>
+      <c r="E25" s="91">
+        <f t="shared" ref="E25:M25" si="15">E10-SUM(E13,E14,E18,E19,E20,E21,E22)</f>
+        <v>-114908780.9132483</v>
+      </c>
+      <c r="F25" s="91">
+        <f t="shared" si="15"/>
+        <v>-21697173.868547082</v>
+      </c>
+      <c r="G25" s="91">
+        <f t="shared" si="15"/>
+        <v>71478973.056824803</v>
+      </c>
+      <c r="H25" s="91">
+        <f t="shared" si="15"/>
+        <v>164619127.96107709</v>
+      </c>
+      <c r="I25" s="91">
+        <f t="shared" si="15"/>
+        <v>424994209.43999988</v>
+      </c>
+      <c r="J25" s="91">
+        <f t="shared" si="15"/>
+        <v>520569824.43999988</v>
+      </c>
+      <c r="K25" s="91">
+        <f t="shared" si="15"/>
+        <v>616145439.43999982</v>
+      </c>
+      <c r="L25" s="91">
+        <f t="shared" si="15"/>
+        <v>711721054.43999982</v>
+      </c>
+      <c r="M25" s="91">
+        <f t="shared" si="15"/>
+        <v>807296669.43999982</v>
       </c>
       <c r="Q25" s="61" t="s">
         <v>1</v>
@@ -4014,10 +4014,10 @@
         <f>SUM(AC16:AC24)</f>
         <v>7679200</v>
       </c>
-      <c r="AN25" s="146" t="s">
+      <c r="AN25" s="113" t="s">
         <v>169</v>
       </c>
-      <c r="AO25" s="147">
+      <c r="AO25" s="114">
         <f>SUM(AO5:AO24)</f>
         <v>404172000</v>
       </c>
@@ -4026,49 +4026,49 @@
       <c r="B26" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="125">
+      <c r="C26" s="92">
         <f>C25</f>
         <v>369912992</v>
       </c>
-      <c r="D26" s="125">
+      <c r="D26" s="92">
         <f>D25+C26</f>
-        <v>163005667.96389329</v>
-      </c>
-      <c r="E26" s="125">
-        <f t="shared" ref="E26:M26" si="10">E25+D26</f>
-        <v>49344887.050644994</v>
-      </c>
-      <c r="F26" s="125">
-        <f t="shared" si="10"/>
-        <v>28895713.182097912</v>
-      </c>
-      <c r="G26" s="125">
-        <f t="shared" si="10"/>
-        <v>101622686.23892272</v>
-      </c>
-      <c r="H26" s="125">
-        <f t="shared" si="10"/>
-        <v>267489814.19999981</v>
-      </c>
-      <c r="I26" s="125">
-        <f t="shared" si="10"/>
-        <v>693732023.63999963</v>
-      </c>
-      <c r="J26" s="125">
-        <f t="shared" si="10"/>
-        <v>1215549848.0799994</v>
-      </c>
-      <c r="K26" s="125">
-        <f t="shared" si="10"/>
-        <v>1832943287.5199993</v>
-      </c>
-      <c r="L26" s="125">
-        <f t="shared" si="10"/>
-        <v>2545912341.9599991</v>
-      </c>
-      <c r="M26" s="125">
-        <f t="shared" si="10"/>
-        <v>3354457011.3999987</v>
+        <v>161757667.96389329</v>
+      </c>
+      <c r="E26" s="92">
+        <f t="shared" ref="E26:M26" si="16">E25+D26</f>
+        <v>46848887.050644994</v>
+      </c>
+      <c r="F26" s="92">
+        <f t="shared" si="16"/>
+        <v>25151713.182097912</v>
+      </c>
+      <c r="G26" s="92">
+        <f t="shared" si="16"/>
+        <v>96630686.238922715</v>
+      </c>
+      <c r="H26" s="92">
+        <f t="shared" si="16"/>
+        <v>261249814.19999981</v>
+      </c>
+      <c r="I26" s="92">
+        <f t="shared" si="16"/>
+        <v>686244023.63999963</v>
+      </c>
+      <c r="J26" s="92">
+        <f t="shared" si="16"/>
+        <v>1206813848.0799994</v>
+      </c>
+      <c r="K26" s="92">
+        <f t="shared" si="16"/>
+        <v>1822959287.5199993</v>
+      </c>
+      <c r="L26" s="92">
+        <f t="shared" si="16"/>
+        <v>2534680341.9599991</v>
+      </c>
+      <c r="M26" s="92">
+        <f t="shared" si="16"/>
+        <v>3341977011.3999987</v>
       </c>
       <c r="Q26" s="61" t="s">
         <v>92</v>
@@ -4096,13 +4096,13 @@
         <f>PMT($U$37,$U$33,-$R$29)</f>
         <v>167271458.4761067</v>
       </c>
-      <c r="Y26" s="99" t="s">
+      <c r="Y26" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="Z26" s="100"/>
-      <c r="AA26" s="100"/>
-      <c r="AB26" s="100"/>
-      <c r="AC26" s="101"/>
+      <c r="Z26" s="123"/>
+      <c r="AA26" s="123"/>
+      <c r="AB26" s="123"/>
+      <c r="AC26" s="124"/>
     </row>
     <row r="27" spans="2:48" x14ac:dyDescent="0.3">
       <c r="Q27" s="61" t="s">
@@ -4148,16 +4148,16 @@
       </c>
     </row>
     <row r="28" spans="2:48" ht="18" x14ac:dyDescent="0.35">
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="132" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="117"/>
-      <c r="I28" s="118"/>
+      <c r="C28" s="133"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="133"/>
+      <c r="G28" s="133"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="134"/>
       <c r="K28" s="81" t="s">
         <v>107</v>
       </c>
@@ -4206,8 +4206,8 @@
         <f>SUM(AA28:AB28)</f>
         <v>579438</v>
       </c>
-      <c r="AH28" s="144"/>
-      <c r="AI28" s="143"/>
+      <c r="AH28" s="111"/>
+      <c r="AI28" s="110"/>
     </row>
     <row r="29" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B29" s="65" t="s">
@@ -4290,27 +4290,27 @@
         <v>85</v>
       </c>
       <c r="C30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" ref="C30:H30" si="17">$AC$13/$C$36</f>
         <v>2916233.3333333335</v>
       </c>
       <c r="D30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" si="17"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="E30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" si="17"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="F30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" si="17"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="G30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" si="17"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="H30" s="14">
-        <f>$AC$13/$C$36</f>
+        <f t="shared" si="17"/>
         <v>2916233.3333333335</v>
       </c>
       <c r="I30" s="15">
@@ -4365,31 +4365,31 @@
         <v>86</v>
       </c>
       <c r="C31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" ref="C31:I31" si="18">$AC$25/$C$35</f>
         <v>1097028.5714285714</v>
       </c>
       <c r="D31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="E31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="F31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="G31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="H31" s="20">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="I31" s="64">
-        <f>$AC$25/$C$35</f>
+        <f t="shared" si="18"/>
         <v>1097028.5714285714</v>
       </c>
       <c r="Y31" s="9"/>
@@ -4404,25 +4404,25 @@
       </c>
     </row>
     <row r="32" spans="2:48" ht="18" x14ac:dyDescent="0.35">
-      <c r="Q32" s="97" t="s">
+      <c r="Q32" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="R32" s="98"/>
-      <c r="T32" s="97" t="s">
+      <c r="R32" s="116"/>
+      <c r="T32" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="U32" s="98"/>
+      <c r="U32" s="116"/>
     </row>
     <row r="33" spans="2:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="B33" s="97" t="s">
+      <c r="B33" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="105"/>
-      <c r="D33" s="98"/>
-      <c r="K33" s="97" t="s">
+      <c r="C33" s="117"/>
+      <c r="D33" s="116"/>
+      <c r="K33" s="115" t="s">
         <v>113</v>
       </c>
-      <c r="L33" s="98"/>
+      <c r="L33" s="116"/>
       <c r="Q33" s="16" t="s">
         <v>95</v>
       </c>
@@ -4562,11 +4562,8 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="AE3:AO3"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="Q24:W24"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:M3"/>
     <mergeCell ref="B24:M24"/>
     <mergeCell ref="Y26:AC26"/>
     <mergeCell ref="Y3:AC3"/>
@@ -4579,8 +4576,11 @@
     <mergeCell ref="B5:M5"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="Y14:AC14"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="AE3:AO3"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="Q24:W24"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:M26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Flujo de caja terminado emprendimiento
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Desarrollo del emprendimiento/Proyecto ABpro Nª2/assets/Flujo de caja.xlsx
+++ b/trabajos.inacap.2019/Desarrollo del emprendimiento/Proyecto ABpro Nª2/assets/Flujo de caja.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C43CE-D874-45E8-9165-B63CBA568A3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58E9E3E-3E63-42C7-B49E-1F63D0828516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="161">
   <si>
     <t>Determinacion de los flujos de efectivo</t>
   </si>
@@ -459,9 +459,6 @@
     <t>Fecha de termino extraordinario</t>
   </si>
   <si>
-    <t>Evaluacion Financiera de VA-RV (Vision artificial para reconocimiento vehicular) a 10 años a partir de 07/05/2019</t>
-  </si>
-  <si>
     <t>Anual</t>
   </si>
   <si>
@@ -494,12 +491,6 @@
     <t xml:space="preserve">Costos de desarrollo Metodologia Scrum Ciclo de vida Prototype - Vision Artificial Para Reconocimiento Vehicular </t>
   </si>
   <si>
-    <t>Carta Gantt</t>
-  </si>
-  <si>
-    <t>Actividad</t>
-  </si>
-  <si>
     <t>Scrum Master</t>
   </si>
   <si>
@@ -518,66 +509,6 @@
     <t>Jefe de programacion</t>
   </si>
   <si>
-    <t>Inicio</t>
-  </si>
-  <si>
-    <t>Fin</t>
-  </si>
-  <si>
-    <t>Definicion de proyecto</t>
-  </si>
-  <si>
-    <t>Planeacion de proyecto</t>
-  </si>
-  <si>
-    <t>Investigacion de factibilidad</t>
-  </si>
-  <si>
-    <t>Recopilacion de requerimientos</t>
-  </si>
-  <si>
-    <t>Iteracion 1 sobre los requerimientos</t>
-  </si>
-  <si>
-    <t>Iteracion 1 sobre la programacion</t>
-  </si>
-  <si>
-    <t>Iteracion 2 sobre la programacion</t>
-  </si>
-  <si>
-    <t>Iteracion 2 sobre los requerimientos</t>
-  </si>
-  <si>
-    <t>Iteracion 3 sobre la programacion</t>
-  </si>
-  <si>
-    <t>Iteracion 3 sobre los requerimientos</t>
-  </si>
-  <si>
-    <t>Iteracion 4 sobre la programacion</t>
-  </si>
-  <si>
-    <t>Iteracion 1 de pruebas</t>
-  </si>
-  <si>
-    <t>Iteracion 4 de pruebas</t>
-  </si>
-  <si>
-    <t>Iteracion 3 de pruebas</t>
-  </si>
-  <si>
-    <t>Iteracion 2 de pruebas</t>
-  </si>
-  <si>
-    <t>Fase de implementacion</t>
-  </si>
-  <si>
-    <t>fase de marcha blanca</t>
-  </si>
-  <si>
-    <t>Inicio de mantencion</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -603,19 +534,56 @@
   </si>
   <si>
     <t>Notebook Acer Swift 3 14"</t>
+  </si>
+  <si>
+    <t>Indicadores financieros</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>TIR</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>Tasa</t>
+  </si>
+  <si>
+    <t>Periodo (Años)</t>
+  </si>
+  <si>
+    <t>Valor libro</t>
+  </si>
+  <si>
+    <t>Flujo efectivo contra inversion</t>
+  </si>
+  <si>
+    <t>Evaluacion Financiera de VA-RV (Vision artificial para reconocimiento vehicular) a 10 años</t>
+  </si>
+  <si>
+    <t>PRI años</t>
+  </si>
+  <si>
+    <t>PRI meses</t>
+  </si>
+  <si>
+    <t>PRI dias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000000%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,14 +714,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -786,7 +746,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,11 +824,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
@@ -1122,7 +1077,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1140,11 +1095,10 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1226,63 +1180,54 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="17" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="19" fillId="6" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="18" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="15" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="16" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="17" xfId="19" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="15" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="16" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="17" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="13" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="16" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="2" fillId="17" borderId="17" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="18" fillId="6" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="10" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="12" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="17" xfId="18" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="16" borderId="15" xfId="18" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="16" borderId="16" xfId="18" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="16" borderId="17" xfId="18" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="13" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="16" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="2" fillId="16" borderId="17" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="16"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="8" applyFont="1"/>
-    <xf numFmtId="42" fontId="19" fillId="6" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="8" applyFont="1"/>
+    <xf numFmtId="42" fontId="18" fillId="6" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
@@ -1312,7 +1257,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1351,22 +1305,25 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="18" fillId="6" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="19">
     <cellStyle name="20% - Énfasis1" xfId="9" builtinId="30"/>
-    <cellStyle name="20% - Énfasis2" xfId="19" builtinId="34"/>
+    <cellStyle name="20% - Énfasis2" xfId="18" builtinId="34"/>
     <cellStyle name="20% - Énfasis4" xfId="12" builtinId="42"/>
     <cellStyle name="20% - Énfasis6" xfId="14" builtinId="50"/>
     <cellStyle name="40% - Énfasis2" xfId="11" builtinId="35"/>
@@ -1374,8 +1331,7 @@
     <cellStyle name="60% - Énfasis4" xfId="13" builtinId="44"/>
     <cellStyle name="60% - Énfasis6" xfId="15" builtinId="52"/>
     <cellStyle name="Bueno" xfId="4" builtinId="26"/>
-    <cellStyle name="Énfasis1" xfId="17" builtinId="29"/>
-    <cellStyle name="Énfasis2" xfId="18" builtinId="33"/>
+    <cellStyle name="Énfasis2" xfId="17" builtinId="33"/>
     <cellStyle name="Entrada" xfId="7" builtinId="20"/>
     <cellStyle name="Hipervínculo" xfId="16" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="5" builtinId="27"/>
@@ -1386,7 +1342,57 @@
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
     <cellStyle name="Salida" xfId="8" builtinId="21"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1688,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AY38"/>
+  <dimension ref="B2:AY55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1699,10 +1705,10 @@
     <col min="2" max="2" width="31.109375" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="16.109375" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" customWidth="1"/>
@@ -1727,7 +1733,7 @@
     <col min="32" max="32" width="24.33203125" customWidth="1"/>
     <col min="33" max="33" width="18.88671875" customWidth="1"/>
     <col min="34" max="34" width="20.88671875" customWidth="1"/>
-    <col min="35" max="35" width="30.21875" customWidth="1"/>
+    <col min="35" max="35" width="28.5546875" customWidth="1"/>
     <col min="36" max="36" width="27.5546875" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
     <col min="38" max="38" width="17.44140625" customWidth="1"/>
@@ -1738,7 +1744,7 @@
     <col min="43" max="43" width="10.33203125" customWidth="1"/>
     <col min="44" max="44" width="12.109375" customWidth="1"/>
     <col min="45" max="45" width="13.77734375" customWidth="1"/>
-    <col min="46" max="46" width="34.6640625" customWidth="1"/>
+    <col min="46" max="46" width="11.44140625" customWidth="1"/>
     <col min="47" max="47" width="13.88671875" customWidth="1"/>
     <col min="48" max="48" width="15.5546875" customWidth="1"/>
     <col min="49" max="49" width="12.5546875" customWidth="1"/>
@@ -1747,65 +1753,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B2" s="144" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="144"/>
+      <c r="B2" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
       <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="2:51" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="145" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="147"/>
-      <c r="Q3" s="115" t="s">
+      <c r="B3" s="111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="113"/>
+      <c r="Q3" s="126" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="116"/>
-      <c r="Y3" s="125" t="s">
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="128"/>
+      <c r="Y3" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="126"/>
-      <c r="AA3" s="126"/>
-      <c r="AB3" s="126"/>
-      <c r="AC3" s="127"/>
-      <c r="AE3" s="115" t="s">
-        <v>134</v>
-      </c>
-      <c r="AF3" s="117"/>
-      <c r="AG3" s="117"/>
-      <c r="AH3" s="117"/>
-      <c r="AI3" s="117"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="117"/>
-      <c r="AL3" s="117"/>
-      <c r="AM3" s="117"/>
-      <c r="AN3" s="117"/>
-      <c r="AO3" s="116"/>
-      <c r="AT3" s="118" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU3" s="118"/>
-      <c r="AV3" s="118"/>
+      <c r="Z3" s="121"/>
+      <c r="AA3" s="121"/>
+      <c r="AB3" s="121"/>
+      <c r="AC3" s="122"/>
+      <c r="AE3" s="126" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF3" s="127"/>
+      <c r="AG3" s="127"/>
+      <c r="AH3" s="127"/>
+      <c r="AI3" s="127"/>
+      <c r="AJ3" s="127"/>
+      <c r="AK3" s="127"/>
+      <c r="AL3" s="127"/>
+      <c r="AM3" s="127"/>
+      <c r="AN3" s="127"/>
+      <c r="AO3" s="128"/>
+      <c r="AT3" s="149"/>
+      <c r="AU3" s="149"/>
+      <c r="AV3" s="149"/>
     </row>
     <row r="4" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1845,7 +1849,7 @@
         <v>10</v>
       </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="87" t="s">
+      <c r="Q4" s="85" t="s">
         <v>17</v>
       </c>
       <c r="R4" s="22" t="s">
@@ -1857,77 +1861,68 @@
       <c r="T4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="88" t="s">
+      <c r="U4" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="Y4" s="128" t="s">
+      <c r="Y4" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="129"/>
-      <c r="AA4" s="129"/>
-      <c r="AB4" s="129"/>
-      <c r="AC4" s="130"/>
-      <c r="AE4" s="94" t="s">
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="125"/>
+      <c r="AE4" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="AF4" s="94" t="s">
+      <c r="AF4" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="AG4" s="94" t="s">
+      <c r="AG4" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="AH4" s="94" t="s">
+      <c r="AH4" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="AI4" s="94" t="s">
+      <c r="AI4" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="AJ4" s="94" t="s">
-        <v>167</v>
-      </c>
-      <c r="AK4" s="94" t="s">
+      <c r="AJ4" s="90" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK4" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="AL4" s="94" t="s">
+      <c r="AL4" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="AM4" s="94" t="s">
-        <v>168</v>
-      </c>
-      <c r="AN4" s="94" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO4" s="94" t="s">
+      <c r="AM4" s="90" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN4" s="90" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO4" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="AT4" s="89" t="s">
-        <v>136</v>
-      </c>
-      <c r="AU4" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="AV4" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="90"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="87"/>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="137"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="135"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="8" t="s">
         <v>7</v>
@@ -1961,47 +1956,38 @@
       <c r="AC5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AE5" s="98" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF5" s="98" t="s">
-        <v>137</v>
-      </c>
-      <c r="AG5" s="101">
+      <c r="AE5" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF5" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG5" s="97">
         <v>43538</v>
       </c>
-      <c r="AH5" s="101">
+      <c r="AH5" s="97">
         <v>43827</v>
       </c>
-      <c r="AI5" s="98"/>
-      <c r="AJ5" s="98">
+      <c r="AI5" s="94"/>
+      <c r="AJ5" s="94">
         <v>7</v>
       </c>
-      <c r="AK5" s="98">
+      <c r="AK5" s="94">
         <v>6</v>
       </c>
-      <c r="AL5" s="95">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="98">
+      <c r="AL5" s="91">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="94">
         <f>((AH5-AG5)*6)+AL5</f>
         <v>1734</v>
       </c>
-      <c r="AN5" s="105">
+      <c r="AN5" s="101">
         <v>17000</v>
       </c>
-      <c r="AO5" s="104">
+      <c r="AO5" s="100">
         <f>AM5*AN5</f>
         <v>29478000</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU5" s="93">
-        <v>43538</v>
-      </c>
-      <c r="AV5" s="93">
-        <v>43545</v>
       </c>
     </row>
     <row r="6" spans="2:51" x14ac:dyDescent="0.3">
@@ -2010,7 +1996,7 @@
       </c>
       <c r="C6" s="74">
         <f>U36</f>
-        <v>800000000</v>
+        <v>550000000</v>
       </c>
       <c r="D6" s="74">
         <v>0</v>
@@ -2067,53 +2053,44 @@
         <v>969990</v>
       </c>
       <c r="AB6" s="26">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="AC6" s="39">
         <f t="shared" ref="AC6:AC12" si="1">AA6*AB6</f>
-        <v>3879960</v>
-      </c>
-      <c r="AE6" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF6" s="99" t="s">
-        <v>138</v>
-      </c>
-      <c r="AG6" s="102">
+        <v>11639880</v>
+      </c>
+      <c r="AE6" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF6" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG6" s="98">
         <v>43539</v>
       </c>
-      <c r="AH6" s="102">
+      <c r="AH6" s="98">
         <v>43827</v>
       </c>
-      <c r="AI6" s="99"/>
-      <c r="AJ6" s="99">
+      <c r="AI6" s="95"/>
+      <c r="AJ6" s="95">
         <v>7</v>
       </c>
-      <c r="AK6" s="99">
+      <c r="AK6" s="95">
         <v>6</v>
       </c>
-      <c r="AL6" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="99">
+      <c r="AL6" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="95">
         <f t="shared" ref="AM6:AM24" si="2">((AH6-AG6)*6)+AL6</f>
         <v>1728</v>
       </c>
-      <c r="AN6" s="106">
+      <c r="AN6" s="102">
         <v>16500</v>
       </c>
-      <c r="AO6" s="108">
+      <c r="AO6" s="104">
         <f t="shared" ref="AO6:AO24" si="3">AM6*AN6</f>
         <v>28512000</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU6" s="93">
-        <v>43525</v>
-      </c>
-      <c r="AV6" s="93">
-        <v>43532</v>
       </c>
     </row>
     <row r="7" spans="2:51" x14ac:dyDescent="0.3">
@@ -2124,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="6">
-        <f>$L$34/10</f>
+        <f>$C$51/10</f>
         <v>1540.3</v>
       </c>
       <c r="E7" s="6">
@@ -2165,7 +2142,7 @@
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R7" s="13">
         <v>137967.19</v>
@@ -2194,47 +2171,38 @@
         <f t="shared" si="1"/>
         <v>86990</v>
       </c>
-      <c r="AE7" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF7" s="99" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG7" s="102">
+      <c r="AE7" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF7" s="95" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG7" s="98">
         <v>43560</v>
       </c>
-      <c r="AH7" s="102">
+      <c r="AH7" s="98">
         <v>43827</v>
       </c>
-      <c r="AI7" s="99"/>
-      <c r="AJ7" s="99">
+      <c r="AI7" s="95"/>
+      <c r="AJ7" s="95">
         <v>7</v>
       </c>
-      <c r="AK7" s="99">
+      <c r="AK7" s="95">
         <v>6</v>
       </c>
-      <c r="AL7" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="99">
+      <c r="AL7" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="95">
         <f t="shared" si="2"/>
         <v>1602</v>
       </c>
-      <c r="AN7" s="106">
+      <c r="AN7" s="102">
         <v>15000</v>
       </c>
-      <c r="AO7" s="108">
+      <c r="AO7" s="104">
         <f t="shared" si="3"/>
         <v>24030000</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AU7" s="93">
-        <v>43533</v>
-      </c>
-      <c r="AV7" s="93">
-        <v>43559</v>
       </c>
     </row>
     <row r="8" spans="2:51" x14ac:dyDescent="0.3">
@@ -2242,48 +2210,48 @@
         <v>110</v>
       </c>
       <c r="C8" s="17">
-        <f t="shared" ref="C8:M8" si="5">$L$29*C7</f>
+        <f>$C$46*C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="17">
-        <f t="shared" si="5"/>
-        <v>130925500</v>
+        <f>$C$46*D7</f>
+        <v>231045000</v>
       </c>
       <c r="E8" s="17">
-        <f t="shared" si="5"/>
-        <v>261851000</v>
+        <f>$C$46*E7</f>
+        <v>462090000</v>
       </c>
       <c r="F8" s="17">
-        <f t="shared" si="5"/>
-        <v>392776499.99999994</v>
+        <f>$C$46*F7</f>
+        <v>693135000</v>
       </c>
       <c r="G8" s="17">
-        <f t="shared" si="5"/>
-        <v>523702000</v>
+        <f>$C$46*G7</f>
+        <v>924180000</v>
       </c>
       <c r="H8" s="17">
-        <f t="shared" si="5"/>
-        <v>654627500</v>
+        <f>$C$46*H7</f>
+        <v>1155225000</v>
       </c>
       <c r="I8" s="17">
-        <f t="shared" si="5"/>
-        <v>785552999.99999988</v>
+        <f>$C$46*I7</f>
+        <v>1386270000</v>
       </c>
       <c r="J8" s="17">
-        <f t="shared" si="5"/>
-        <v>916478499.99999988</v>
+        <f>$C$46*J7</f>
+        <v>1617314999.9999998</v>
       </c>
       <c r="K8" s="17">
-        <f t="shared" si="5"/>
-        <v>1047403999.9999998</v>
+        <f>$C$46*K7</f>
+        <v>1848359999.9999998</v>
       </c>
       <c r="L8" s="17">
-        <f t="shared" si="5"/>
-        <v>1178329499.9999998</v>
+        <f>$C$46*L7</f>
+        <v>2079404999.9999995</v>
       </c>
       <c r="M8" s="76">
-        <f t="shared" si="5"/>
-        <v>1309254999.9999998</v>
+        <f>$C$46*M7</f>
+        <v>2310449999.9999995</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="16" t="s">
@@ -2310,53 +2278,44 @@
         <v>145490</v>
       </c>
       <c r="AB8" s="26">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="AC8" s="39">
         <f t="shared" si="1"/>
-        <v>581960</v>
-      </c>
-      <c r="AE8" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF8" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG8" s="102">
+        <v>1745880</v>
+      </c>
+      <c r="AE8" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF8" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG8" s="98">
         <v>43588</v>
       </c>
-      <c r="AH8" s="102">
+      <c r="AH8" s="98">
         <v>43827</v>
       </c>
-      <c r="AI8" s="99"/>
-      <c r="AJ8" s="99">
+      <c r="AI8" s="95"/>
+      <c r="AJ8" s="95">
         <v>7</v>
       </c>
-      <c r="AK8" s="99">
+      <c r="AK8" s="95">
         <v>6</v>
       </c>
-      <c r="AL8" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="99">
+      <c r="AL8" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN8" s="106">
+      <c r="AN8" s="102">
         <v>14000</v>
       </c>
-      <c r="AO8" s="108">
+      <c r="AO8" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU8" s="93">
-        <v>43560</v>
-      </c>
-      <c r="AV8" s="93">
-        <v>43595</v>
       </c>
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.3">
@@ -2369,43 +2328,43 @@
       </c>
       <c r="D9" s="77">
         <f>D8</f>
-        <v>130925500</v>
+        <v>231045000</v>
       </c>
       <c r="E9" s="77">
-        <f t="shared" ref="E9:M9" si="6">E8</f>
-        <v>261851000</v>
+        <f t="shared" ref="E9:M9" si="5">E8</f>
+        <v>462090000</v>
       </c>
       <c r="F9" s="77">
-        <f t="shared" si="6"/>
-        <v>392776499.99999994</v>
+        <f t="shared" si="5"/>
+        <v>693135000</v>
       </c>
       <c r="G9" s="77">
-        <f t="shared" si="6"/>
-        <v>523702000</v>
+        <f t="shared" si="5"/>
+        <v>924180000</v>
       </c>
       <c r="H9" s="77">
-        <f t="shared" si="6"/>
-        <v>654627500</v>
+        <f t="shared" si="5"/>
+        <v>1155225000</v>
       </c>
       <c r="I9" s="77">
-        <f t="shared" si="6"/>
-        <v>785552999.99999988</v>
+        <f t="shared" si="5"/>
+        <v>1386270000</v>
       </c>
       <c r="J9" s="77">
-        <f t="shared" si="6"/>
-        <v>916478499.99999988</v>
+        <f t="shared" si="5"/>
+        <v>1617314999.9999998</v>
       </c>
       <c r="K9" s="77">
-        <f t="shared" si="6"/>
-        <v>1047403999.9999998</v>
+        <f t="shared" si="5"/>
+        <v>1848359999.9999998</v>
       </c>
       <c r="L9" s="77">
-        <f t="shared" si="6"/>
-        <v>1178329499.9999998</v>
+        <f t="shared" si="5"/>
+        <v>2079404999.9999995</v>
       </c>
       <c r="M9" s="78">
-        <f t="shared" si="6"/>
-        <v>1309254999.9999998</v>
+        <f t="shared" si="5"/>
+        <v>2310449999.9999995</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="16" t="s">
@@ -2438,47 +2397,38 @@
         <f t="shared" si="1"/>
         <v>279090</v>
       </c>
-      <c r="AE9" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF9" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG9" s="102">
+      <c r="AE9" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF9" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG9" s="98">
         <v>43588</v>
       </c>
-      <c r="AH9" s="102">
+      <c r="AH9" s="98">
         <v>43827</v>
       </c>
-      <c r="AI9" s="99"/>
-      <c r="AJ9" s="99">
+      <c r="AI9" s="95"/>
+      <c r="AJ9" s="95">
         <v>7</v>
       </c>
-      <c r="AK9" s="99">
+      <c r="AK9" s="95">
         <v>6</v>
       </c>
-      <c r="AL9" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="99">
+      <c r="AL9" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN9" s="106">
+      <c r="AN9" s="102">
         <v>14000</v>
       </c>
-      <c r="AO9" s="108">
+      <c r="AO9" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>150</v>
-      </c>
-      <c r="AU9" s="93">
-        <v>43596</v>
-      </c>
-      <c r="AV9" s="93">
-        <v>43617</v>
       </c>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.3">
@@ -2489,44 +2439,44 @@
         <v>0</v>
       </c>
       <c r="D10" s="79">
-        <f t="shared" ref="D10:M10" si="7">D9-(D9*$L$38)</f>
-        <v>95575615</v>
+        <f>D9-(D9*$C$55)</f>
+        <v>168662850</v>
       </c>
       <c r="E10" s="79">
-        <f t="shared" si="7"/>
-        <v>191151230</v>
+        <f>E9-(E9*$C$55)</f>
+        <v>337325700</v>
       </c>
       <c r="F10" s="79">
-        <f t="shared" si="7"/>
-        <v>286726844.99999994</v>
+        <f>F9-(F9*$C$55)</f>
+        <v>505988550</v>
       </c>
       <c r="G10" s="79">
-        <f t="shared" si="7"/>
-        <v>382302460</v>
+        <f>G9-(G9*$C$55)</f>
+        <v>674651400</v>
       </c>
       <c r="H10" s="79">
-        <f t="shared" si="7"/>
-        <v>477878075</v>
+        <f>H9-(H9*$C$55)</f>
+        <v>843314250</v>
       </c>
       <c r="I10" s="79">
-        <f t="shared" si="7"/>
-        <v>573453689.99999988</v>
+        <f>I9-(I9*$C$55)</f>
+        <v>1011977100</v>
       </c>
       <c r="J10" s="79">
-        <f t="shared" si="7"/>
-        <v>669029304.99999988</v>
+        <f>J9-(J9*$C$55)</f>
+        <v>1180639949.9999998</v>
       </c>
       <c r="K10" s="79">
-        <f t="shared" si="7"/>
-        <v>764604919.99999976</v>
+        <f>K9-(K9*$C$55)</f>
+        <v>1349302799.9999998</v>
       </c>
       <c r="L10" s="79">
-        <f t="shared" si="7"/>
-        <v>860180534.99999976</v>
+        <f>L9-(L9*$C$55)</f>
+        <v>1517965649.9999995</v>
       </c>
       <c r="M10" s="80">
-        <f t="shared" si="7"/>
-        <v>955756149.99999976</v>
+        <f>M9-(M9*$C$55)</f>
+        <v>1686628499.9999995</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="16" t="s">
@@ -2559,47 +2509,38 @@
         <f t="shared" si="1"/>
         <v>99800</v>
       </c>
-      <c r="AE10" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF10" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG10" s="102">
+      <c r="AE10" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF10" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG10" s="98">
         <v>43588</v>
       </c>
-      <c r="AH10" s="102">
+      <c r="AH10" s="98">
         <v>43827</v>
       </c>
-      <c r="AI10" s="99"/>
-      <c r="AJ10" s="99">
+      <c r="AI10" s="95"/>
+      <c r="AJ10" s="95">
         <v>7</v>
       </c>
-      <c r="AK10" s="99">
+      <c r="AK10" s="95">
         <v>6</v>
       </c>
-      <c r="AL10" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="99">
+      <c r="AL10" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN10" s="106">
+      <c r="AN10" s="102">
         <v>14000</v>
       </c>
-      <c r="AO10" s="108">
+      <c r="AO10" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>156</v>
-      </c>
-      <c r="AU10" s="93">
-        <v>43618</v>
-      </c>
-      <c r="AV10" s="93">
-        <v>43623</v>
       </c>
     </row>
     <row r="11" spans="2:51" x14ac:dyDescent="0.3">
@@ -2619,80 +2560,71 @@
         <v>94990</v>
       </c>
       <c r="AB11" s="26">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC11" s="39">
         <f t="shared" si="1"/>
-        <v>1899800</v>
-      </c>
-      <c r="AE11" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF11" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG11" s="102">
+        <v>1994790</v>
+      </c>
+      <c r="AE11" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF11" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG11" s="98">
         <v>43588</v>
       </c>
-      <c r="AH11" s="102">
+      <c r="AH11" s="98">
         <v>43827</v>
       </c>
-      <c r="AI11" s="99"/>
-      <c r="AJ11" s="99">
+      <c r="AI11" s="95"/>
+      <c r="AJ11" s="95">
         <v>7</v>
       </c>
-      <c r="AK11" s="99">
+      <c r="AK11" s="95">
         <v>6</v>
       </c>
-      <c r="AL11" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="99">
+      <c r="AL11" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN11" s="106">
+      <c r="AN11" s="102">
         <v>14000</v>
       </c>
-      <c r="AO11" s="108">
+      <c r="AO11" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU11" s="93">
-        <v>43624</v>
-      </c>
-      <c r="AV11" s="93">
-        <v>8</v>
-      </c>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="139"/>
-      <c r="L12" s="139"/>
-      <c r="M12" s="140"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="137"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="137"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="138"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="7"/>
       <c r="Y12" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z12" s="112" t="s">
-        <v>170</v>
+        <v>148</v>
+      </c>
+      <c r="Z12" s="26" t="s">
+        <v>147</v>
       </c>
       <c r="AA12" s="38">
         <v>533490</v>
@@ -2704,47 +2636,38 @@
         <f t="shared" si="1"/>
         <v>10669800</v>
       </c>
-      <c r="AE12" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF12" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG12" s="102">
+      <c r="AE12" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF12" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG12" s="98">
         <v>43588</v>
       </c>
-      <c r="AH12" s="102">
+      <c r="AH12" s="98">
         <v>43827</v>
       </c>
-      <c r="AI12" s="99"/>
-      <c r="AJ12" s="99">
+      <c r="AI12" s="95"/>
+      <c r="AJ12" s="95">
         <v>7</v>
       </c>
-      <c r="AK12" s="99">
+      <c r="AK12" s="95">
         <v>6</v>
       </c>
-      <c r="AL12" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="99">
+      <c r="AL12" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN12" s="106">
+      <c r="AN12" s="102">
         <v>14000</v>
       </c>
-      <c r="AO12" s="108">
+      <c r="AO12" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT12" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU12" s="93">
-        <v>43625</v>
-      </c>
-      <c r="AV12" s="93">
-        <v>43645</v>
       </c>
     </row>
     <row r="13" spans="2:51" x14ac:dyDescent="0.3">
@@ -2759,54 +2682,54 @@
         <v>145495480.56</v>
       </c>
       <c r="E13" s="74">
-        <f t="shared" ref="E13:M13" si="8">$U$5*12</f>
+        <f t="shared" ref="E13:M13" si="6">$U$5*12</f>
         <v>145495480.56</v>
       </c>
       <c r="F13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="G13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="H13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="I13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="J13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="K13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="L13" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
       <c r="M13" s="75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>145495480.56</v>
       </c>
-      <c r="Q13" s="85" t="s">
+      <c r="Q13" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="83" t="s">
+      <c r="R13" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="S13" s="83" t="s">
+      <c r="S13" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="T13" s="83" t="s">
+      <c r="T13" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="U13" s="84" t="s">
+      <c r="U13" s="82" t="s">
         <v>19</v>
       </c>
       <c r="Y13" s="8"/>
@@ -2817,49 +2740,40 @@
       </c>
       <c r="AC13" s="39">
         <f>SUM(AC6:AC12)</f>
-        <v>17497400</v>
-      </c>
-      <c r="AE13" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF13" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG13" s="102">
+        <v>26516230</v>
+      </c>
+      <c r="AE13" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF13" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG13" s="98">
         <v>43588</v>
       </c>
-      <c r="AH13" s="102">
+      <c r="AH13" s="98">
         <v>43827</v>
       </c>
-      <c r="AI13" s="99"/>
-      <c r="AJ13" s="99">
+      <c r="AI13" s="95"/>
+      <c r="AJ13" s="95">
         <v>7</v>
       </c>
-      <c r="AK13" s="99">
+      <c r="AK13" s="95">
         <v>6</v>
       </c>
-      <c r="AL13" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="99">
+      <c r="AL13" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN13" s="106">
+      <c r="AN13" s="102">
         <v>14000</v>
       </c>
-      <c r="AO13" s="108">
+      <c r="AO13" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT13" t="s">
-        <v>159</v>
-      </c>
-      <c r="AU13" s="93">
-        <v>43646</v>
-      </c>
-      <c r="AV13" s="93">
-        <v>43651</v>
       </c>
     </row>
     <row r="14" spans="2:51" x14ac:dyDescent="0.3">
@@ -2870,43 +2784,43 @@
         <v>12</v>
       </c>
       <c r="D14" s="17">
-        <f t="shared" ref="D14:M14" si="9">$U$14*12</f>
+        <f t="shared" ref="D14:M14" si="7">$U$14*12</f>
         <v>2964000</v>
       </c>
       <c r="E14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="F14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="G14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="H14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="I14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="J14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="K14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="L14" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="M14" s="76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2964000</v>
       </c>
       <c r="Q14" s="16" t="s">
@@ -2922,58 +2836,49 @@
         <f>(R14*S14)+R14</f>
         <v>156000</v>
       </c>
-      <c r="U14" s="86">
+      <c r="U14" s="84">
         <f>SUM(T14:T15)</f>
         <v>247000</v>
       </c>
-      <c r="Y14" s="141" t="s">
+      <c r="Y14" s="139" t="s">
         <v>42</v>
       </c>
-      <c r="Z14" s="142"/>
-      <c r="AA14" s="142"/>
-      <c r="AB14" s="142"/>
-      <c r="AC14" s="143"/>
-      <c r="AE14" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF14" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG14" s="102">
+      <c r="Z14" s="140"/>
+      <c r="AA14" s="140"/>
+      <c r="AB14" s="140"/>
+      <c r="AC14" s="141"/>
+      <c r="AE14" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF14" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG14" s="98">
         <v>43588</v>
       </c>
-      <c r="AH14" s="102">
+      <c r="AH14" s="98">
         <v>43827</v>
       </c>
-      <c r="AI14" s="99"/>
-      <c r="AJ14" s="99">
+      <c r="AI14" s="95"/>
+      <c r="AJ14" s="95">
         <v>7</v>
       </c>
-      <c r="AK14" s="99">
+      <c r="AK14" s="95">
         <v>6</v>
       </c>
-      <c r="AL14" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="99">
+      <c r="AL14" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN14" s="106">
+      <c r="AN14" s="102">
         <v>14000</v>
       </c>
-      <c r="AO14" s="108">
+      <c r="AO14" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU14" s="93">
-        <v>43652</v>
-      </c>
-      <c r="AV14" s="93">
-        <v>43652</v>
       </c>
     </row>
     <row r="15" spans="2:51" x14ac:dyDescent="0.3">
@@ -2984,28 +2889,28 @@
         <v>12</v>
       </c>
       <c r="D15" s="17">
-        <f t="shared" ref="D15:I15" si="10">$AC$13/6</f>
-        <v>2916233.3333333335</v>
+        <f t="shared" ref="D15:I15" si="8">$AC$13/6</f>
+        <v>4419371.666666667</v>
       </c>
       <c r="E15" s="17">
-        <f t="shared" si="10"/>
-        <v>2916233.3333333335</v>
+        <f t="shared" si="8"/>
+        <v>4419371.666666667</v>
       </c>
       <c r="F15" s="17">
-        <f t="shared" si="10"/>
-        <v>2916233.3333333335</v>
+        <f t="shared" si="8"/>
+        <v>4419371.666666667</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="10"/>
-        <v>2916233.3333333335</v>
+        <f t="shared" si="8"/>
+        <v>4419371.666666667</v>
       </c>
       <c r="H15" s="17">
-        <f t="shared" si="10"/>
-        <v>2916233.3333333335</v>
+        <f t="shared" si="8"/>
+        <v>4419371.666666667</v>
       </c>
       <c r="I15" s="17">
-        <f t="shared" si="10"/>
-        <v>2916233.3333333335</v>
+        <f t="shared" si="8"/>
+        <v>4419371.666666667</v>
       </c>
       <c r="J15" s="17">
         <v>0</v>
@@ -3029,7 +2934,7 @@
         <v>0.3</v>
       </c>
       <c r="T15" s="13">
-        <f t="shared" ref="T15" si="11">(R15*S15)+R15</f>
+        <f t="shared" ref="T15" si="9">(R15*S15)+R15</f>
         <v>91000</v>
       </c>
       <c r="U15" s="7"/>
@@ -3048,47 +2953,38 @@
       <c r="AC15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="AE15" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF15" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG15" s="102">
+      <c r="AE15" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF15" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG15" s="98">
         <v>43588</v>
       </c>
-      <c r="AH15" s="102">
+      <c r="AH15" s="98">
         <v>43827</v>
       </c>
-      <c r="AI15" s="99"/>
-      <c r="AJ15" s="99">
+      <c r="AI15" s="95"/>
+      <c r="AJ15" s="95">
         <v>7</v>
       </c>
-      <c r="AK15" s="99">
+      <c r="AK15" s="95">
         <v>6</v>
       </c>
-      <c r="AL15" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM15" s="99">
+      <c r="AL15" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN15" s="106">
+      <c r="AN15" s="102">
         <v>14000</v>
       </c>
-      <c r="AO15" s="108">
+      <c r="AO15" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
-      </c>
-      <c r="AT15" t="s">
-        <v>153</v>
-      </c>
-      <c r="AU15" s="93">
-        <v>43653</v>
-      </c>
-      <c r="AV15" s="93">
-        <v>43676</v>
       </c>
     </row>
     <row r="16" spans="2:51" x14ac:dyDescent="0.3">
@@ -3099,32 +2995,32 @@
         <v>12</v>
       </c>
       <c r="D16" s="17">
-        <f t="shared" ref="D16:J16" si="12">$AC$25/7</f>
-        <v>1097028.5714285714</v>
+        <f t="shared" ref="D16:J16" si="10">$AC$25/7</f>
+        <v>1268451.4285714286</v>
       </c>
       <c r="E16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="F16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="G16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="H16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="I16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="J16" s="17">
-        <f t="shared" si="12"/>
-        <v>1097028.5714285714</v>
+        <f t="shared" si="10"/>
+        <v>1268451.4285714286</v>
       </c>
       <c r="K16" s="17">
         <v>0</v>
@@ -3156,50 +3052,41 @@
         <f>AA16*AB16</f>
         <v>1639800</v>
       </c>
-      <c r="AE16" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF16" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG16" s="102">
+      <c r="AE16" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF16" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG16" s="98">
         <v>43588</v>
       </c>
-      <c r="AH16" s="102">
+      <c r="AH16" s="98">
         <v>43827</v>
       </c>
-      <c r="AI16" s="99"/>
-      <c r="AJ16" s="99">
+      <c r="AI16" s="95"/>
+      <c r="AJ16" s="95">
         <v>7</v>
       </c>
-      <c r="AK16" s="99">
+      <c r="AK16" s="95">
         <v>6</v>
       </c>
-      <c r="AL16" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="99">
+      <c r="AL16" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN16" s="106">
+      <c r="AN16" s="102">
         <v>14000</v>
       </c>
-      <c r="AO16" s="108">
+      <c r="AO16" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT16" t="s">
-        <v>158</v>
-      </c>
-      <c r="AU16" s="93">
-        <v>43677</v>
-      </c>
-      <c r="AV16" s="93">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="17" spans="2:48" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
@@ -3207,24 +3094,24 @@
         <v>12</v>
       </c>
       <c r="D17" s="17">
-        <f t="shared" ref="D17:H18" si="13">S27</f>
-        <v>12000000</v>
+        <f t="shared" ref="D17:H18" si="11">S27</f>
+        <v>8250000</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" si="13"/>
-        <v>9670928.1228583995</v>
+        <f t="shared" si="11"/>
+        <v>6648763.0844651489</v>
       </c>
       <c r="F17" s="17">
-        <f t="shared" si="13"/>
-        <v>7306920.1675596759</v>
+        <f t="shared" si="11"/>
+        <v>5023507.6151972758</v>
       </c>
       <c r="G17" s="17">
-        <f t="shared" si="13"/>
-        <v>4907452.0929314708</v>
+        <f t="shared" si="11"/>
+        <v>3373873.3138903845</v>
       </c>
       <c r="H17" s="17">
-        <f t="shared" si="13"/>
-        <v>2471991.9971838421</v>
+        <f t="shared" si="11"/>
+        <v>1699494.49806389</v>
       </c>
       <c r="I17" s="17">
         <v>0</v>
@@ -3262,50 +3149,41 @@
         <f>AA17*AB17</f>
         <v>1599800</v>
       </c>
-      <c r="AE17" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF17" s="99" t="s">
-        <v>164</v>
-      </c>
-      <c r="AG17" s="102">
-        <v>43588</v>
-      </c>
-      <c r="AH17" s="102">
+      <c r="AE17" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF17" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG17" s="98">
+        <v>43560</v>
+      </c>
+      <c r="AH17" s="98">
         <v>43827</v>
       </c>
-      <c r="AI17" s="99"/>
-      <c r="AJ17" s="99">
+      <c r="AI17" s="95"/>
+      <c r="AJ17" s="95">
         <v>7</v>
       </c>
-      <c r="AK17" s="99">
+      <c r="AK17" s="95">
         <v>6</v>
       </c>
-      <c r="AL17" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="99">
+      <c r="AL17" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="95">
         <f t="shared" si="2"/>
-        <v>1434</v>
-      </c>
-      <c r="AN17" s="106">
+        <v>1602</v>
+      </c>
+      <c r="AN17" s="102">
         <v>15000</v>
       </c>
-      <c r="AO17" s="108">
+      <c r="AO17" s="104">
         <f t="shared" si="3"/>
-        <v>21510000</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU17" s="93">
-        <v>43683</v>
-      </c>
-      <c r="AV17" s="93">
-        <v>43683</v>
-      </c>
-    </row>
-    <row r="18" spans="2:48" x14ac:dyDescent="0.3">
+        <v>24030000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
@@ -3313,24 +3191,24 @@
         <v>12</v>
       </c>
       <c r="D18" s="17">
-        <f t="shared" si="13"/>
-        <v>155271458.4761067</v>
+        <f t="shared" si="11"/>
+        <v>106749127.70232336</v>
       </c>
       <c r="E18" s="17">
-        <f t="shared" si="13"/>
-        <v>157600530.3532483</v>
+        <f t="shared" si="11"/>
+        <v>108350364.61785822</v>
       </c>
       <c r="F18" s="17">
-        <f t="shared" si="13"/>
-        <v>159964538.30854702</v>
+        <f t="shared" si="11"/>
+        <v>109975620.08712609</v>
       </c>
       <c r="G18" s="17">
-        <f t="shared" si="13"/>
-        <v>162364006.38317522</v>
+        <f t="shared" si="11"/>
+        <v>111625254.38843298</v>
       </c>
       <c r="H18" s="17">
-        <f t="shared" si="13"/>
-        <v>164799466.47892287</v>
+        <f t="shared" si="11"/>
+        <v>113299633.20425947</v>
       </c>
       <c r="I18" s="17">
         <v>0</v>
@@ -3362,62 +3240,53 @@
         <v>299990</v>
       </c>
       <c r="AB18" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC18" s="42">
         <f>AA18*AB18</f>
-        <v>599980</v>
-      </c>
-      <c r="AE18" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF18" s="99" t="s">
-        <v>163</v>
-      </c>
-      <c r="AG18" s="102">
+        <v>899970</v>
+      </c>
+      <c r="AE18" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF18" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG18" s="98">
         <v>43588</v>
       </c>
-      <c r="AH18" s="102">
+      <c r="AH18" s="98">
         <v>43827</v>
       </c>
-      <c r="AI18" s="99"/>
-      <c r="AJ18" s="99">
+      <c r="AI18" s="95"/>
+      <c r="AJ18" s="95">
         <v>7</v>
       </c>
-      <c r="AK18" s="99">
+      <c r="AK18" s="95">
         <v>6</v>
       </c>
-      <c r="AL18" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="99">
+      <c r="AL18" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN18" s="106">
+      <c r="AN18" s="102">
         <v>14000</v>
       </c>
-      <c r="AO18" s="108">
+      <c r="AO18" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AU18" s="93">
-        <v>43684</v>
-      </c>
-      <c r="AV18" s="93">
-        <v>43707</v>
-      </c>
-    </row>
-    <row r="19" spans="2:48" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="17">
         <f>AO25</f>
-        <v>404172000</v>
+        <v>409212000</v>
       </c>
       <c r="D19" s="17">
         <v>0</v>
@@ -3464,62 +3333,53 @@
         <v>29990</v>
       </c>
       <c r="AB19" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC19" s="42">
-        <f t="shared" ref="AC19:AC21" si="14">AA19*AB19</f>
-        <v>59980</v>
-      </c>
-      <c r="AE19" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF19" s="99" t="s">
-        <v>163</v>
-      </c>
-      <c r="AG19" s="102">
+        <f t="shared" ref="AC19:AC21" si="12">AA19*AB19</f>
+        <v>89970</v>
+      </c>
+      <c r="AE19" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF19" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG19" s="98">
         <v>43588</v>
       </c>
-      <c r="AH19" s="102">
+      <c r="AH19" s="98">
         <v>43827</v>
       </c>
-      <c r="AI19" s="99"/>
-      <c r="AJ19" s="99">
+      <c r="AI19" s="95"/>
+      <c r="AJ19" s="95">
         <v>7</v>
       </c>
-      <c r="AK19" s="99">
+      <c r="AK19" s="95">
         <v>6</v>
       </c>
-      <c r="AL19" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="99">
+      <c r="AL19" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN19" s="106">
+      <c r="AN19" s="102">
         <v>14000</v>
       </c>
-      <c r="AO19" s="108">
+      <c r="AO19" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT19" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU19" s="93">
-        <v>43708</v>
-      </c>
-      <c r="AV19" s="93">
-        <v>43718</v>
-      </c>
-    </row>
-    <row r="20" spans="2:48" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="17">
         <f>AC13</f>
-        <v>17497400</v>
+        <v>26516230</v>
       </c>
       <c r="D20" s="17">
         <v>0</v>
@@ -3569,150 +3429,132 @@
         <v>8</v>
       </c>
       <c r="AC20" s="42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>639920</v>
       </c>
-      <c r="AE20" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF20" s="99" t="s">
-        <v>165</v>
-      </c>
-      <c r="AG20" s="102">
+      <c r="AE20" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF20" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG20" s="98">
+        <v>43560</v>
+      </c>
+      <c r="AH20" s="98">
+        <v>43827</v>
+      </c>
+      <c r="AI20" s="95"/>
+      <c r="AJ20" s="95">
+        <v>7</v>
+      </c>
+      <c r="AK20" s="95">
+        <v>6</v>
+      </c>
+      <c r="AL20" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="95">
+        <f t="shared" si="2"/>
+        <v>1602</v>
+      </c>
+      <c r="AN20" s="102">
+        <v>15000</v>
+      </c>
+      <c r="AO20" s="104">
+        <f t="shared" si="3"/>
+        <v>24030000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="17">
+        <f>AC25</f>
+        <v>8879160</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0</v>
+      </c>
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="17">
+        <v>0</v>
+      </c>
+      <c r="M21" s="76">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z21" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA21" s="41">
+        <v>69990</v>
+      </c>
+      <c r="AB21" s="30">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="42">
+        <f t="shared" si="12"/>
+        <v>209970</v>
+      </c>
+      <c r="AE21" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF21" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG21" s="98">
         <v>43588</v>
       </c>
-      <c r="AH20" s="102">
+      <c r="AH21" s="98">
         <v>43827</v>
       </c>
-      <c r="AI20" s="99"/>
-      <c r="AJ20" s="99">
+      <c r="AI21" s="95"/>
+      <c r="AJ21" s="95">
         <v>7</v>
       </c>
-      <c r="AK20" s="99">
+      <c r="AK21" s="95">
         <v>6</v>
       </c>
-      <c r="AL20" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="99">
+      <c r="AL21" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN20" s="106">
-        <v>15000</v>
-      </c>
-      <c r="AO20" s="108">
-        <f t="shared" si="3"/>
-        <v>21510000</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>160</v>
-      </c>
-      <c r="AU20" s="93">
-        <v>43719</v>
-      </c>
-      <c r="AV20" s="93">
-        <v>43748</v>
-      </c>
-    </row>
-    <row r="21" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="17">
-        <f>AC25</f>
-        <v>7679200</v>
-      </c>
-      <c r="D21" s="17">
-        <v>0</v>
-      </c>
-      <c r="E21" s="17">
-        <v>0</v>
-      </c>
-      <c r="F21" s="17">
-        <v>0</v>
-      </c>
-      <c r="G21" s="17">
-        <v>0</v>
-      </c>
-      <c r="H21" s="17">
-        <v>0</v>
-      </c>
-      <c r="I21" s="17">
-        <v>0</v>
-      </c>
-      <c r="J21" s="17">
-        <v>0</v>
-      </c>
-      <c r="K21" s="17">
-        <v>0</v>
-      </c>
-      <c r="L21" s="17">
-        <v>0</v>
-      </c>
-      <c r="M21" s="76">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z21" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA21" s="41">
-        <v>69990</v>
-      </c>
-      <c r="AB21" s="30">
-        <v>2</v>
-      </c>
-      <c r="AC21" s="42">
-        <f t="shared" si="14"/>
-        <v>139980</v>
-      </c>
-      <c r="AE21" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF21" s="99" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG21" s="102">
-        <v>43588</v>
-      </c>
-      <c r="AH21" s="102">
-        <v>43827</v>
-      </c>
-      <c r="AI21" s="99"/>
-      <c r="AJ21" s="99">
-        <v>7</v>
-      </c>
-      <c r="AK21" s="99">
-        <v>6</v>
-      </c>
-      <c r="AL21" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="99">
-        <f t="shared" si="2"/>
-        <v>1434</v>
-      </c>
-      <c r="AN21" s="106">
+      <c r="AN21" s="102">
         <v>14000</v>
       </c>
-      <c r="AO21" s="108">
+      <c r="AO21" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT21" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU21" s="93">
-        <v>43749</v>
-      </c>
-      <c r="AV21" s="93">
-        <v>43827</v>
-      </c>
-    </row>
-    <row r="22" spans="2:48" ht="23.4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="2:41" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B22" s="9" t="s">
         <v>91</v>
       </c>
@@ -3750,10 +3592,10 @@
       <c r="M22" s="68">
         <v>0</v>
       </c>
-      <c r="Q22" s="131" t="s">
+      <c r="Q22" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="R22" s="131"/>
+      <c r="R22" s="129"/>
       <c r="Y22" s="40" t="s">
         <v>55</v>
       </c>
@@ -3764,53 +3606,47 @@
         <v>799990</v>
       </c>
       <c r="AB22" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC22" s="42">
         <f>AA22*AB22</f>
-        <v>1599980</v>
-      </c>
-      <c r="AE22" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF22" s="99" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG22" s="102">
+        <v>2399970</v>
+      </c>
+      <c r="AE22" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF22" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG22" s="98">
         <v>43588</v>
       </c>
-      <c r="AH22" s="102">
+      <c r="AH22" s="98">
         <v>43827</v>
       </c>
-      <c r="AI22" s="99"/>
-      <c r="AJ22" s="99">
+      <c r="AI22" s="95"/>
+      <c r="AJ22" s="95">
         <v>7</v>
       </c>
-      <c r="AK22" s="99">
+      <c r="AK22" s="95">
         <v>6</v>
       </c>
-      <c r="AL22" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="99">
+      <c r="AL22" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="95">
         <f t="shared" si="2"/>
         <v>1434</v>
       </c>
-      <c r="AN22" s="106">
+      <c r="AN22" s="102">
         <v>14000</v>
       </c>
-      <c r="AO22" s="108">
+      <c r="AO22" s="104">
         <f t="shared" si="3"/>
         <v>20076000</v>
       </c>
-      <c r="AT22" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU22" s="93">
-        <v>43828</v>
-      </c>
-    </row>
-    <row r="23" spans="2:48" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:41" x14ac:dyDescent="0.3">
       <c r="Y23" s="40" t="s">
         <v>57</v>
       </c>
@@ -3827,64 +3663,64 @@
         <f>AA23*AB23</f>
         <v>799960</v>
       </c>
-      <c r="AE23" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF23" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG23" s="102">
+      <c r="AE23" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF23" s="95" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG23" s="98">
         <v>43719</v>
       </c>
-      <c r="AH23" s="102">
+      <c r="AH23" s="98">
         <v>43827</v>
       </c>
-      <c r="AI23" s="99"/>
-      <c r="AJ23" s="99">
+      <c r="AI23" s="95"/>
+      <c r="AJ23" s="95">
         <v>7</v>
       </c>
-      <c r="AK23" s="99">
+      <c r="AK23" s="95">
         <v>6</v>
       </c>
-      <c r="AL23" s="96">
-        <v>0</v>
-      </c>
-      <c r="AM23" s="99">
+      <c r="AL23" s="92">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="95">
         <f t="shared" si="2"/>
         <v>648</v>
       </c>
-      <c r="AN23" s="106">
+      <c r="AN23" s="102">
         <v>14000</v>
       </c>
-      <c r="AO23" s="108">
+      <c r="AO23" s="104">
         <f t="shared" si="3"/>
         <v>9072000</v>
       </c>
     </row>
-    <row r="24" spans="2:48" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="119" t="s">
+    <row r="24" spans="2:41" ht="18" x14ac:dyDescent="0.35">
+      <c r="B24" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="120"/>
-      <c r="I24" s="120"/>
-      <c r="J24" s="120"/>
-      <c r="K24" s="120"/>
-      <c r="L24" s="120"/>
-      <c r="M24" s="121"/>
-      <c r="Q24" s="115" t="s">
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="115"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="115"/>
+      <c r="L24" s="115"/>
+      <c r="M24" s="116"/>
+      <c r="Q24" s="126" t="s">
         <v>103</v>
       </c>
-      <c r="R24" s="117"/>
-      <c r="S24" s="117"/>
-      <c r="T24" s="117"/>
-      <c r="U24" s="117"/>
-      <c r="V24" s="117"/>
-      <c r="W24" s="116"/>
+      <c r="R24" s="127"/>
+      <c r="S24" s="127"/>
+      <c r="T24" s="127"/>
+      <c r="U24" s="127"/>
+      <c r="V24" s="127"/>
+      <c r="W24" s="128"/>
       <c r="Y24" s="40" t="s">
         <v>59</v>
       </c>
@@ -3901,87 +3737,87 @@
         <f>AA24*AB24</f>
         <v>599800</v>
       </c>
-      <c r="AE24" s="100" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF24" s="100" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG24" s="103">
+      <c r="AE24" s="96" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF24" s="96" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG24" s="99">
         <v>43719</v>
       </c>
-      <c r="AH24" s="103">
+      <c r="AH24" s="99">
         <v>43827</v>
       </c>
-      <c r="AI24" s="100"/>
-      <c r="AJ24" s="100">
+      <c r="AI24" s="96"/>
+      <c r="AJ24" s="96">
         <v>7</v>
       </c>
-      <c r="AK24" s="100">
+      <c r="AK24" s="96">
         <v>6</v>
       </c>
-      <c r="AL24" s="97">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="100">
+      <c r="AL24" s="93">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="96">
         <f t="shared" si="2"/>
         <v>648</v>
       </c>
-      <c r="AN24" s="107">
+      <c r="AN24" s="103">
         <v>14000</v>
       </c>
-      <c r="AO24" s="109">
+      <c r="AO24" s="105">
         <f t="shared" si="3"/>
         <v>9072000</v>
       </c>
     </row>
-    <row r="25" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B25" s="50" t="s">
+    <row r="25" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B25" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="91">
+      <c r="C25" s="144">
         <f>C6-C19-C20-C21-C22</f>
-        <v>369912992</v>
-      </c>
-      <c r="D25" s="91">
+        <v>104654202</v>
+      </c>
+      <c r="D25" s="88">
         <f>D10-SUM(D13,D14,D18,D19,D20,D21,D22)</f>
-        <v>-208155324.03610671</v>
-      </c>
-      <c r="E25" s="91">
-        <f t="shared" ref="E25:M25" si="15">E10-SUM(E13,E14,E18,E19,E20,E21,E22)</f>
-        <v>-114908780.9132483</v>
-      </c>
-      <c r="F25" s="91">
-        <f t="shared" si="15"/>
-        <v>-21697173.868547082</v>
-      </c>
-      <c r="G25" s="91">
-        <f t="shared" si="15"/>
-        <v>71478973.056824803</v>
-      </c>
-      <c r="H25" s="91">
-        <f t="shared" si="15"/>
-        <v>164619127.96107709</v>
-      </c>
-      <c r="I25" s="91">
-        <f t="shared" si="15"/>
-        <v>424994209.43999988</v>
-      </c>
-      <c r="J25" s="91">
-        <f t="shared" si="15"/>
-        <v>520569824.43999988</v>
-      </c>
-      <c r="K25" s="91">
-        <f t="shared" si="15"/>
-        <v>616145439.43999982</v>
-      </c>
-      <c r="L25" s="91">
-        <f t="shared" si="15"/>
-        <v>711721054.43999982</v>
-      </c>
-      <c r="M25" s="91">
-        <f t="shared" si="15"/>
-        <v>807296669.43999982</v>
+        <v>-86545758.26232338</v>
+      </c>
+      <c r="E25" s="88">
+        <f t="shared" ref="E25:M25" si="13">E10-SUM(E13,E14,E18,E19,E20,E21,E22)</f>
+        <v>80515854.822141767</v>
+      </c>
+      <c r="F25" s="88">
+        <f t="shared" si="13"/>
+        <v>247553449.35287392</v>
+      </c>
+      <c r="G25" s="88">
+        <f t="shared" si="13"/>
+        <v>414566665.05156702</v>
+      </c>
+      <c r="H25" s="88">
+        <f t="shared" si="13"/>
+        <v>581555136.23574054</v>
+      </c>
+      <c r="I25" s="88">
+        <f t="shared" si="13"/>
+        <v>863517619.44000006</v>
+      </c>
+      <c r="J25" s="88">
+        <f t="shared" si="13"/>
+        <v>1032180469.4399998</v>
+      </c>
+      <c r="K25" s="88">
+        <f t="shared" si="13"/>
+        <v>1200843319.4399998</v>
+      </c>
+      <c r="L25" s="88">
+        <f t="shared" si="13"/>
+        <v>1369506169.4399996</v>
+      </c>
+      <c r="M25" s="88">
+        <f t="shared" si="13"/>
+        <v>1538169019.4399996</v>
       </c>
       <c r="Q25" s="61" t="s">
         <v>1</v>
@@ -4012,63 +3848,63 @@
       </c>
       <c r="AC25" s="42">
         <f>SUM(AC16:AC24)</f>
-        <v>7679200</v>
-      </c>
-      <c r="AN25" s="113" t="s">
-        <v>169</v>
-      </c>
-      <c r="AO25" s="114">
+        <v>8879160</v>
+      </c>
+      <c r="AN25" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="AO25" s="109">
         <f>SUM(AO5:AO24)</f>
-        <v>404172000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B26" s="9" t="s">
+        <v>409212000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B26" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="92">
+      <c r="C26" s="145">
         <f>C25</f>
-        <v>369912992</v>
-      </c>
-      <c r="D26" s="92">
+        <v>104654202</v>
+      </c>
+      <c r="D26" s="89">
         <f>D25+C26</f>
-        <v>161757667.96389329</v>
-      </c>
-      <c r="E26" s="92">
-        <f t="shared" ref="E26:M26" si="16">E25+D26</f>
-        <v>46848887.050644994</v>
-      </c>
-      <c r="F26" s="92">
-        <f t="shared" si="16"/>
-        <v>25151713.182097912</v>
-      </c>
-      <c r="G26" s="92">
-        <f t="shared" si="16"/>
-        <v>96630686.238922715</v>
-      </c>
-      <c r="H26" s="92">
-        <f t="shared" si="16"/>
-        <v>261249814.19999981</v>
-      </c>
-      <c r="I26" s="92">
-        <f t="shared" si="16"/>
-        <v>686244023.63999963</v>
-      </c>
-      <c r="J26" s="92">
-        <f t="shared" si="16"/>
-        <v>1206813848.0799994</v>
-      </c>
-      <c r="K26" s="92">
-        <f t="shared" si="16"/>
-        <v>1822959287.5199993</v>
-      </c>
-      <c r="L26" s="92">
-        <f t="shared" si="16"/>
-        <v>2534680341.9599991</v>
-      </c>
-      <c r="M26" s="92">
-        <f t="shared" si="16"/>
-        <v>3341977011.3999987</v>
+        <v>18108443.73767662</v>
+      </c>
+      <c r="E26" s="89">
+        <f t="shared" ref="E26:M26" si="14">E25+D26</f>
+        <v>98624298.559818387</v>
+      </c>
+      <c r="F26" s="89">
+        <f t="shared" si="14"/>
+        <v>346177747.91269231</v>
+      </c>
+      <c r="G26" s="89">
+        <f t="shared" si="14"/>
+        <v>760744412.96425939</v>
+      </c>
+      <c r="H26" s="89">
+        <f t="shared" si="14"/>
+        <v>1342299549.1999998</v>
+      </c>
+      <c r="I26" s="89">
+        <f t="shared" si="14"/>
+        <v>2205817168.6399999</v>
+      </c>
+      <c r="J26" s="89">
+        <f t="shared" si="14"/>
+        <v>3237997638.0799999</v>
+      </c>
+      <c r="K26" s="89">
+        <f t="shared" si="14"/>
+        <v>4438840957.5199995</v>
+      </c>
+      <c r="L26" s="89">
+        <f t="shared" si="14"/>
+        <v>5808347126.9599991</v>
+      </c>
+      <c r="M26" s="89">
+        <f t="shared" si="14"/>
+        <v>7346516146.3999987</v>
       </c>
       <c r="Q26" s="61" t="s">
         <v>92</v>
@@ -4078,33 +3914,80 @@
       </c>
       <c r="S26" s="62">
         <f>PMT($U$37,$U$33,-$R$29)</f>
-        <v>167271458.4761067</v>
+        <v>114999127.70232336</v>
       </c>
       <c r="T26" s="62">
         <f>PMT($U$37,$U$33,-$R$29)</f>
-        <v>167271458.4761067</v>
+        <v>114999127.70232336</v>
       </c>
       <c r="U26" s="62">
         <f>PMT($U$37,$U$33,-$R$29)</f>
-        <v>167271458.4761067</v>
+        <v>114999127.70232336</v>
       </c>
       <c r="V26" s="62">
         <f>PMT($U$37,$U$33,-$R$29)</f>
-        <v>167271458.4761067</v>
+        <v>114999127.70232336</v>
       </c>
       <c r="W26" s="63">
         <f>PMT($U$37,$U$33,-$R$29)</f>
-        <v>167271458.4761067</v>
-      </c>
-      <c r="Y26" s="122" t="s">
+        <v>114999127.70232336</v>
+      </c>
+      <c r="Y26" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="Z26" s="123"/>
-      <c r="AA26" s="123"/>
-      <c r="AB26" s="123"/>
-      <c r="AC26" s="124"/>
-    </row>
-    <row r="27" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="Z26" s="118"/>
+      <c r="AA26" s="118"/>
+      <c r="AB26" s="118"/>
+      <c r="AC26" s="119"/>
+    </row>
+    <row r="27" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B27" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="145">
+        <f>-U36</f>
+        <v>-550000000</v>
+      </c>
+      <c r="D27" s="145">
+        <f>D25</f>
+        <v>-86545758.26232338</v>
+      </c>
+      <c r="E27" s="145">
+        <f t="shared" ref="E27:M27" si="15">E25</f>
+        <v>80515854.822141767</v>
+      </c>
+      <c r="F27" s="145">
+        <f t="shared" si="15"/>
+        <v>247553449.35287392</v>
+      </c>
+      <c r="G27" s="145">
+        <f t="shared" si="15"/>
+        <v>414566665.05156702</v>
+      </c>
+      <c r="H27" s="145">
+        <f t="shared" si="15"/>
+        <v>581555136.23574054</v>
+      </c>
+      <c r="I27" s="145">
+        <f t="shared" si="15"/>
+        <v>863517619.44000006</v>
+      </c>
+      <c r="J27" s="145">
+        <f t="shared" si="15"/>
+        <v>1032180469.4399998</v>
+      </c>
+      <c r="K27" s="145">
+        <f t="shared" si="15"/>
+        <v>1200843319.4399998</v>
+      </c>
+      <c r="L27" s="145">
+        <f t="shared" si="15"/>
+        <v>1369506169.4399996</v>
+      </c>
+      <c r="M27" s="145">
+        <f t="shared" si="15"/>
+        <v>1538169019.4399996</v>
+      </c>
       <c r="Q27" s="61" t="s">
         <v>23</v>
       </c>
@@ -4113,23 +3996,23 @@
       </c>
       <c r="S27" s="62">
         <f>+R29*$U$37</f>
-        <v>12000000</v>
+        <v>8250000</v>
       </c>
       <c r="T27" s="62">
         <f>+S29*$U$37</f>
-        <v>9670928.1228583995</v>
+        <v>6648763.0844651489</v>
       </c>
       <c r="U27" s="62">
         <f>+T29*$U$37</f>
-        <v>7306920.1675596759</v>
+        <v>5023507.6151972758</v>
       </c>
       <c r="V27" s="62">
         <f>+U29*$U$37</f>
-        <v>4907452.0929314708</v>
+        <v>3373873.3138903845</v>
       </c>
       <c r="W27" s="63">
         <f>+V29*$U$37</f>
-        <v>2471991.9971838421</v>
+        <v>1699494.49806389</v>
       </c>
       <c r="Y27" s="31" t="s">
         <v>17</v>
@@ -4147,21 +4030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:48" ht="18" x14ac:dyDescent="0.35">
-      <c r="B28" s="132" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="134"/>
-      <c r="K28" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="L28" s="82"/>
+    <row r="28" spans="2:41" x14ac:dyDescent="0.3">
       <c r="Q28" s="61" t="s">
         <v>80</v>
       </c>
@@ -4170,23 +4039,23 @@
       </c>
       <c r="S28" s="62">
         <f>+S26-S27</f>
-        <v>155271458.4761067</v>
+        <v>106749127.70232336</v>
       </c>
       <c r="T28" s="62">
         <f>+T26-T27</f>
-        <v>157600530.3532483</v>
+        <v>108350364.61785822</v>
       </c>
       <c r="U28" s="62">
         <f>+U26-U27</f>
-        <v>159964538.30854702</v>
+        <v>109975620.08712609</v>
       </c>
       <c r="V28" s="62">
         <f>+V26-V27</f>
-        <v>162364006.38317522</v>
+        <v>111625254.38843298</v>
       </c>
       <c r="W28" s="63">
         <f>+W26-W27</f>
-        <v>164799466.47892287</v>
+        <v>113299633.20425947</v>
       </c>
       <c r="Y28" s="53" t="s">
         <v>65</v>
@@ -4206,66 +4075,50 @@
         <f>SUM(AA28:AB28)</f>
         <v>579438</v>
       </c>
-      <c r="AH28" s="111"/>
-      <c r="AI28" s="110"/>
-    </row>
-    <row r="29" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B29" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4">
-        <v>2</v>
-      </c>
-      <c r="E29" s="4">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4">
-        <v>4</v>
-      </c>
-      <c r="G29" s="4">
-        <v>5</v>
-      </c>
-      <c r="H29" s="4">
-        <v>6</v>
-      </c>
-      <c r="I29" s="5">
-        <v>7</v>
-      </c>
-      <c r="K29" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="L29" s="69">
-        <v>85000</v>
-      </c>
+      <c r="AH28" s="107"/>
+      <c r="AI28" s="106"/>
+    </row>
+    <row r="29" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B29" s="142" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="142"/>
+      <c r="D29" s="142"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="142"/>
+      <c r="K29" s="142"/>
+      <c r="L29" s="142"/>
+      <c r="M29" s="142"/>
       <c r="Q29" s="61" t="s">
         <v>93</v>
       </c>
       <c r="R29" s="60">
         <f>U36</f>
-        <v>800000000</v>
+        <v>550000000</v>
       </c>
       <c r="S29" s="62">
         <f>+R29-S28</f>
-        <v>644728541.52389336</v>
+        <v>443250872.29767662</v>
       </c>
       <c r="T29" s="62">
         <f>+S29-T28</f>
-        <v>487128011.17064506</v>
+        <v>334900507.67981839</v>
       </c>
       <c r="U29" s="62">
         <f>+T29-U28</f>
-        <v>327163472.86209804</v>
+        <v>224924887.59269232</v>
       </c>
       <c r="V29" s="62">
         <f>+U29-V28</f>
-        <v>164799466.47892281</v>
+        <v>113299633.20425934</v>
       </c>
       <c r="W29" s="63">
         <f>+V29-W28</f>
-        <v>0</v>
+        <v>-1.3411045074462891E-7</v>
       </c>
       <c r="Y29" s="43" t="s">
         <v>66</v>
@@ -4285,44 +4138,7 @@
         <v>158970</v>
       </c>
     </row>
-    <row r="30" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="14">
-        <f t="shared" ref="C30:H30" si="17">$AC$13/$C$36</f>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="D30" s="14">
-        <f t="shared" si="17"/>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="E30" s="14">
-        <f t="shared" si="17"/>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="F30" s="14">
-        <f t="shared" si="17"/>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="G30" s="14">
-        <f t="shared" si="17"/>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="H30" s="14">
-        <f t="shared" si="17"/>
-        <v>2916233.3333333335</v>
-      </c>
-      <c r="I30" s="15">
-        <v>0</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L30" s="70">
-        <f>L29/1000</f>
-        <v>85</v>
-      </c>
+    <row r="30" spans="2:41" x14ac:dyDescent="0.3">
       <c r="Q30" s="61" t="s">
         <v>94</v>
       </c>
@@ -4331,23 +4147,23 @@
       </c>
       <c r="S30" s="62">
         <f>+S28+R30</f>
-        <v>155271458.4761067</v>
+        <v>106749127.70232336</v>
       </c>
       <c r="T30" s="62">
         <f>+T28+S30</f>
-        <v>312871988.829355</v>
+        <v>215099492.32018158</v>
       </c>
       <c r="U30" s="62">
         <f>+U28+T30</f>
-        <v>472836527.13790202</v>
+        <v>325075112.40730768</v>
       </c>
       <c r="V30" s="62">
         <f>+V28+U30</f>
-        <v>635200533.52107728</v>
+        <v>436700366.79574066</v>
       </c>
       <c r="W30" s="63">
         <f>+W28+V30</f>
-        <v>800000000.00000012</v>
+        <v>550000000.00000012</v>
       </c>
       <c r="Y30" s="8"/>
       <c r="Z30" s="6"/>
@@ -4360,38 +4176,7 @@
         <v>738408</v>
       </c>
     </row>
-    <row r="31" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="20">
-        <f t="shared" ref="C31:I31" si="18">$AC$25/$C$35</f>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="D31" s="20">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="E31" s="20">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="F31" s="20">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="G31" s="20">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="H31" s="20">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
-      <c r="I31" s="64">
-        <f t="shared" si="18"/>
-        <v>1097028.5714285714</v>
-      </c>
+    <row r="31" spans="2:41" x14ac:dyDescent="0.3">
       <c r="Y31" s="9"/>
       <c r="Z31" s="10"/>
       <c r="AA31" s="10"/>
@@ -4400,29 +4185,54 @@
       </c>
       <c r="AC31" s="59">
         <f>SUM(AC30,AC25,AC13)</f>
-        <v>25915008</v>
-      </c>
-    </row>
-    <row r="32" spans="2:48" ht="18" x14ac:dyDescent="0.35">
-      <c r="Q32" s="115" t="s">
+        <v>36133798</v>
+      </c>
+    </row>
+    <row r="32" spans="2:41" ht="18" x14ac:dyDescent="0.35">
+      <c r="B32" s="130" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="131"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="131"/>
+      <c r="F32" s="131"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="131"/>
+      <c r="I32" s="132"/>
+      <c r="Q32" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="R32" s="116"/>
-      <c r="T32" s="115" t="s">
+      <c r="R32" s="128"/>
+      <c r="T32" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="U32" s="116"/>
-    </row>
-    <row r="33" spans="2:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="B33" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="117"/>
-      <c r="D33" s="116"/>
-      <c r="K33" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="L33" s="116"/>
+      <c r="U32" s="128"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B33" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4">
+        <v>6</v>
+      </c>
+      <c r="I33" s="5">
+        <v>7</v>
+      </c>
       <c r="Q33" s="16" t="s">
         <v>95</v>
       </c>
@@ -4437,20 +4247,35 @@
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B34" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="L34" s="69">
-        <v>15403</v>
+      <c r="B34" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*C33)</f>
+        <v>22096858.333333332</v>
+      </c>
+      <c r="D34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*D33)</f>
+        <v>17677486.666666664</v>
+      </c>
+      <c r="E34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*E33)</f>
+        <v>13258115</v>
+      </c>
+      <c r="F34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*F33)</f>
+        <v>8838743.3333333321</v>
+      </c>
+      <c r="G34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*G33)</f>
+        <v>4419371.6666666642</v>
+      </c>
+      <c r="H34" s="14">
+        <f>$AC$13-(($AC$13/$C$40)*H33)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="84">
+        <v>0</v>
       </c>
       <c r="Q34" s="16" t="s">
         <v>97</v>
@@ -4462,25 +4287,42 @@
         <v>80</v>
       </c>
       <c r="U34" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B35" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="48">
-        <v>7</v>
-      </c>
-      <c r="D35" s="47">
-        <v>2</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="L35" s="57">
-        <v>16396</v>
-      </c>
+      <c r="B35" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*C33)</f>
+        <v>7610708.5714285709</v>
+      </c>
+      <c r="D35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*D33)</f>
+        <v>6342257.1428571427</v>
+      </c>
+      <c r="E35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*E33)</f>
+        <v>5073805.7142857146</v>
+      </c>
+      <c r="F35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*F33)</f>
+        <v>3805354.2857142854</v>
+      </c>
+      <c r="G35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*G33)</f>
+        <v>2536902.8571428563</v>
+      </c>
+      <c r="H35" s="20">
+        <f>$AC$25-(($AC$25/$C$39)*H33)</f>
+        <v>1268451.4285714282</v>
+      </c>
+      <c r="I35" s="64">
+        <f>$AC$25-(($AC$25/$C$39)*I33)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="106"/>
       <c r="Q35" s="16" t="s">
         <v>98</v>
       </c>
@@ -4495,21 +4337,6 @@
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B36" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="45">
-        <v>6</v>
-      </c>
-      <c r="D36" s="45">
-        <v>2</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="L36" s="70">
-        <v>126049</v>
-      </c>
       <c r="Q36" s="16" t="s">
         <v>99</v>
       </c>
@@ -4520,10 +4347,19 @@
         <v>101</v>
       </c>
       <c r="U36" s="15">
-        <v>800000000</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
+        <v>550000000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="B37" s="126" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="127"/>
+      <c r="D37" s="128"/>
+      <c r="F37" s="126" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" s="128"/>
       <c r="Q37" s="16" t="s">
         <v>100</v>
       </c>
@@ -4538,14 +4374,20 @@
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B38" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L38" s="73">
-        <v>0.27</v>
+      <c r="B38" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="143">
+        <v>0.25</v>
       </c>
       <c r="Q38" s="67" t="s">
         <v>112</v>
@@ -4560,29 +4402,199 @@
         <v>118</v>
       </c>
     </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B39" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="48">
+        <v>7</v>
+      </c>
+      <c r="D39" s="47">
+        <v>2</v>
+      </c>
+      <c r="F39" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B40" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="45">
+        <v>6</v>
+      </c>
+      <c r="D40" s="45">
+        <v>2</v>
+      </c>
+      <c r="F40" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="84">
+        <f>NPV(G38,D25:M25)-U36</f>
+        <v>912681020.93063402</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F41" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="146">
+        <f>IRR(C27:M27)</f>
+        <v>0.454655924331129</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B42" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="7">
+        <f>(D4+((U36-D26)/E25))</f>
+        <v>7.6060474354679997</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F43" s="45"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="45" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="B45" s="126" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="128"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B46" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="147">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="148">
+        <f>C46/1000</f>
+        <v>150</v>
+      </c>
+      <c r="F47" s="152" t="s">
+        <v>158</v>
+      </c>
+      <c r="G47" s="150">
+        <f>ROUNDDOWN(G42,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F48" s="153" t="s">
+        <v>159</v>
+      </c>
+      <c r="G48" s="7">
+        <f>ROUNDDOWN(((G42-ROUNDDOWN(G42,0))*12),0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F49" s="154" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" s="151">
+        <f>(((G42-ROUNDDOWN(G42,0))*12)-ROUNDDOWN(((G42-ROUNDDOWN(G42,0))*12),0))*30</f>
+        <v>8.1770767684798784</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B50" s="126" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="128"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="69">
+        <v>15403</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="57">
+        <v>16396</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="70">
+        <v>126049</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="73">
+        <v>0.27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="AE3:AO3"/>
+    <mergeCell ref="Q24:W24"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="T32:U32"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B24:M24"/>
     <mergeCell ref="Y26:AC26"/>
     <mergeCell ref="Y3:AC3"/>
     <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B12:M12"/>
     <mergeCell ref="Y14:AC14"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="AE3:AO3"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="Q24:W24"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:M26">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N44:P44">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:M27">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>